<commit_message>
correct DOF in tests, correct misleading formatting of operational case study
</commit_message>
<xml_diff>
--- a/pareto/case_studies/operational_generic_case_study.xlsx
+++ b/pareto/case_studies/operational_generic_case_study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89492181-180C-49F8-A1C4-AA7CF2F5EB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AC5AEE-63BA-4278-BFF3-85719F40EF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14445" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="770" firstSheet="34" activeTab="41" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="770" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -74,172 +74,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Andres Calderon</author>
-  </authors>
-  <commentList>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{99618F5E-9634-421E-A41A-271BAE2797D1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This value is added as "clutter" for testing purposes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{DAF72A8D-E948-4544-A79F-2A2DB092DF89}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Contains white spaces for testing purposes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{B3BE548B-9451-4ACE-845C-1C70635761A5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Cell with some calculations for testing purposes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{D5A71132-39A3-4638-9D45-CAE15CC160EB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Contains white spaces for testing purposes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{875F4A7E-B8F1-4274-9617-5F7FC3688FD8}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This value is added as "clutter" for testing purposes</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Andres Calderon</author>
-  </authors>
-  <commentList>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{D285F83C-4D6A-4221-AB67-25E4DE633D02}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This cell used to contain data that was deleted. This was a common source of errors when using get_data()</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="152">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -509,12 +345,6 @@
   </si>
   <si>
     <t>Production Pads to Treatment Facilities Trucking Arcs [-]</t>
-  </si>
-  <si>
-    <t>PROPRIETARY DATA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     </t>
   </si>
   <si>
     <t xml:space="preserve">    </t>
@@ -710,7 +540,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -777,19 +607,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -797,7 +614,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -813,12 +630,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1258,9 +1069,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1339,7 +1150,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1358,54 +1168,54 @@
     <xf numFmtId="43" fontId="3" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="3" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1793,7 +1603,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2442,7 +2252,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2453,37 +2263,31 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="36"/>
+        <v>102</v>
+      </c>
+      <c r="B3" s="36"/>
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
-        <v>105</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
+        <v>103</v>
+      </c>
+      <c r="B4" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2492,14 +2296,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2512,18 +2316,19 @@
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="39" t="s">
-        <v>90</v>
-      </c>
+      <c r="B1" s="39"/>
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -2532,11 +2337,8 @@
       <c r="B3" s="36">
         <v>1</v>
       </c>
-      <c r="E3" s="40">
-        <v>1</v>
-      </c>
-      <c r="F3" s="40" t="s">
-        <v>92</v>
+      <c r="F3" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2546,36 +2348,14 @@
       <c r="B4" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="40">
-        <f>1+1/2+1/3+1/4</f>
-        <v>2.083333333333333</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D8" s="40">
-        <v>1</v>
-      </c>
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2633,7 +2413,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2646,13 +2426,11 @@
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="39" t="s">
-        <v>90</v>
-      </c>
+      <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -2699,9 +2477,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D9" s="39" t="s">
-        <v>90</v>
-      </c>
+      <c r="D9" s="39"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2711,14 +2487,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED7A596-FF30-4282-98C8-7AB378F1FE03}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED7A596-FF30-4282-98C8-7AB378F1FE03}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2733,7 +2509,7 @@
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -2754,12 +2530,11 @@
       <c r="B4" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="40"/>
+      <c r="D4" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2786,7 +2561,7 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -2830,7 +2605,7 @@
     </row>
     <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>54</v>
@@ -2924,276 +2699,276 @@
   <sheetData>
     <row r="1" spans="1:52" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:52" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="E2" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="51"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="50"/>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="E3" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="G3" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="H3" s="56"/>
+      <c r="I3" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="F3" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="G3" s="56" t="s">
+      <c r="K3" s="57" t="s">
         <v>119</v>
-      </c>
-      <c r="H3" s="57"/>
-      <c r="I3" s="56" t="s">
-        <v>120</v>
-      </c>
-      <c r="J3" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="K3" s="58" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="52" t="s">
         <v>122</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="E4" s="53" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="F4" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="E4" s="54" t="s">
-        <v>125</v>
-      </c>
-      <c r="F4" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="G4" s="56" t="s">
-        <v>126</v>
-      </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="58"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="57"/>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="52" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="53" t="s">
-        <v>129</v>
-      </c>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="61"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="60"/>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="E6" s="53" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="53" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="54" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="G6" s="56" t="s">
-        <v>133</v>
-      </c>
-      <c r="H6" s="53"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="61"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="60"/>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="E7" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="F7" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="55" t="s">
         <v>136</v>
       </c>
-      <c r="E7" s="54" t="s">
-        <v>137</v>
-      </c>
-      <c r="F7" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="G7" s="56" t="s">
-        <v>138</v>
-      </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="61"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="60"/>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="52" t="s">
         <v>139</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="E8" s="58"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="60"/>
+      <c r="AT8" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="AU8" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV8" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="AW8" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="AX8" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="AY8" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ8" s="37" t="s">
         <v>140</v>
-      </c>
-      <c r="D8" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="61"/>
-      <c r="AT8" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="AU8" s="37" t="s">
-        <v>122</v>
-      </c>
-      <c r="AV8" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW8" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="AX8" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="AY8" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="AZ8" s="37" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:52" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="61" t="s">
         <v>143</v>
       </c>
-      <c r="B9" s="43" t="s">
-        <v>140</v>
-      </c>
-      <c r="D9" s="62" t="s">
+      <c r="E9" s="62" t="s">
+        <v>144</v>
+      </c>
+      <c r="F9" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="G9" s="64" t="s">
         <v>145</v>
       </c>
-      <c r="E9" s="63" t="s">
+      <c r="H9" s="61"/>
+      <c r="I9" s="65" t="s">
         <v>146</v>
       </c>
-      <c r="F9" s="64" t="s">
-        <v>118</v>
-      </c>
-      <c r="G9" s="65" t="s">
+      <c r="J9" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="K9" s="64" t="s">
         <v>147</v>
       </c>
-      <c r="H9" s="62"/>
-      <c r="I9" s="66" t="s">
+      <c r="AT9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AU9" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="J9" s="64" t="s">
-        <v>118</v>
-      </c>
-      <c r="K9" s="65" t="s">
-        <v>149</v>
-      </c>
-      <c r="AT9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AU9" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="AV9" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="AW9" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AX9" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AY9" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AZ9" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.3">
       <c r="AT10" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AU10" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="AV10" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AW10" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AX10" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AY10" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AZ10" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.3">
       <c r="AU11" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AZ11" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.3">
       <c r="AU12" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AZ12" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -3248,7 +3023,7 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>54</v>
@@ -3292,7 +3067,7 @@
     </row>
     <row r="2" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>61</v>
@@ -3494,7 +3269,7 @@
     </row>
     <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
@@ -3569,10 +3344,10 @@
     </row>
     <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>93</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>95</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>56</v>
@@ -3946,7 +3721,7 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
@@ -4098,7 +3873,7 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
@@ -4169,10 +3944,10 @@
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D2" s="39"/>
     </row>
@@ -4249,7 +4024,7 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
@@ -4339,9 +4114,9 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="40" t="s">
         <v>56</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -4361,19 +4136,19 @@
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3" s="41">
         <v>10000</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="41">
         <v>10000</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="41">
         <v>10000</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="41">
         <v>10000</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="42">
         <v>10000</v>
       </c>
     </row>
@@ -4473,10 +4248,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4539,10 +4314,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4609,10 +4384,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4653,7 +4428,7 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -4706,10 +4481,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4759,9 +4534,9 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="40" t="s">
         <v>56</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -4781,19 +4556,19 @@
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3" s="41">
         <v>250</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="41">
         <v>250</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="41">
         <v>250</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="41">
         <v>250</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="42">
         <v>250</v>
       </c>
     </row>
@@ -4827,10 +4602,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4929,7 +4704,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>3</v>
@@ -5252,20 +5027,20 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="36">
         <v>1</v>
@@ -5273,7 +5048,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
@@ -5310,17 +5085,17 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="67">
+      <c r="B3" s="66">
         <v>142277</v>
       </c>
     </row>
@@ -5328,7 +5103,7 @@
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="68">
+      <c r="B4" s="67">
         <v>140998</v>
       </c>
     </row>
@@ -5336,7 +5111,7 @@
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="68">
+      <c r="B5" s="67">
         <v>172490.2</v>
       </c>
     </row>
@@ -5344,7 +5119,7 @@
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="68">
+      <c r="B6" s="67">
         <v>257547</v>
       </c>
     </row>
@@ -5352,7 +5127,7 @@
       <c r="A7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="68">
+      <c r="B7" s="67">
         <v>241833.8</v>
       </c>
     </row>
@@ -5360,7 +5135,7 @@
       <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="69">
+      <c r="B8" s="68">
         <v>188503.7</v>
       </c>
     </row>
@@ -5377,7 +5152,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5395,15 +5170,15 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="44" t="s">
         <v>107</v>
       </c>
+      <c r="B2" s="43" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5625,12 +5400,12 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>

</xml_diff>

<commit_message>
updating the hydraulics module to address the review comments
</commit_message>
<xml_diff>
--- a/pareto/case_studies/operational_generic_case_study.xlsx
+++ b/pareto/case_studies/operational_generic_case_study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naresh\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89492181-180C-49F8-A1C4-AA7CF2F5EB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AB5981-F847-4E63-92CC-BB42B67223C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14445" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="770" firstSheet="34" activeTab="41" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="770" firstSheet="1" activeTab="1" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -239,7 +239,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="161">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -701,6 +701,27 @@
   </si>
   <si>
     <t>meter</t>
+  </si>
+  <si>
+    <t>pressure</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>Pressure units when using the hydraulics module</t>
+  </si>
+  <si>
+    <t>6895 Pa</t>
+  </si>
+  <si>
+    <t>pascal</t>
+  </si>
+  <si>
+    <t>elevation</t>
+  </si>
+  <si>
+    <t>Elevation of a network node (including all sites)</t>
   </si>
 </sst>
 </file>
@@ -2897,9 +2918,11 @@
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
   </sheetPr>
-  <dimension ref="A1:AZ12"/>
+  <dimension ref="A1:BA12"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2918,16 +2941,17 @@
     <col min="49" max="49" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="16384" width="9.33203125" style="1"/>
+    <col min="52" max="52" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:52" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>111</v>
       </c>
@@ -2947,7 +2971,7 @@
       <c r="J2" s="49"/>
       <c r="K2" s="51"/>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>115</v>
       </c>
@@ -2977,7 +3001,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>122</v>
       </c>
@@ -3001,7 +3025,7 @@
       <c r="J4" s="56"/>
       <c r="K4" s="58"/>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>127</v>
       </c>
@@ -3019,7 +3043,7 @@
       <c r="J5" s="60"/>
       <c r="K5" s="61"/>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>130</v>
       </c>
@@ -3043,7 +3067,7 @@
       <c r="J6" s="60"/>
       <c r="K6" s="61"/>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>134</v>
       </c>
@@ -3067,7 +3091,7 @@
       <c r="J7" s="60"/>
       <c r="K7" s="61"/>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>139</v>
       </c>
@@ -3103,38 +3127,35 @@
         <v>139</v>
       </c>
       <c r="AZ8" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="BA8" s="37" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="B9" s="43" t="s">
-        <v>140</v>
-      </c>
-      <c r="D9" s="62" t="s">
-        <v>145</v>
-      </c>
-      <c r="E9" s="63" t="s">
-        <v>146</v>
-      </c>
-      <c r="F9" s="64" t="s">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="53" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="59" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" s="60" t="s">
         <v>118</v>
       </c>
-      <c r="G9" s="65" t="s">
-        <v>147</v>
-      </c>
-      <c r="H9" s="62"/>
-      <c r="I9" s="66" t="s">
-        <v>148</v>
-      </c>
-      <c r="J9" s="64" t="s">
-        <v>118</v>
-      </c>
-      <c r="K9" s="65" t="s">
-        <v>149</v>
-      </c>
+      <c r="G9" s="60" t="s">
+        <v>157</v>
+      </c>
+      <c r="H9" s="53"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="61"/>
       <c r="AT9" s="1" t="s">
         <v>116</v>
       </c>
@@ -3154,10 +3175,29 @@
         <v>140</v>
       </c>
       <c r="AZ9" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="BA9" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" s="59"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="61"/>
       <c r="AT10" s="1" t="s">
         <v>120</v>
       </c>
@@ -3177,47 +3217,81 @@
         <v>144</v>
       </c>
       <c r="AZ10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="BA10" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="G11" s="65" t="s">
+        <v>147</v>
+      </c>
+      <c r="H11" s="62"/>
+      <c r="I11" s="66" t="s">
+        <v>148</v>
+      </c>
+      <c r="J11" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="K11" s="65" t="s">
+        <v>149</v>
+      </c>
       <c r="AU11" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="AZ11" s="1" t="s">
+      <c r="BA11" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AU12" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="AZ12" s="1" t="s">
+      <c r="BA12" s="1" t="s">
         <v>148</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{983EC2A0-C4EA-4CE0-BED1-203B514C4F46}">
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{86102F73-0552-4E90-BC6E-A014997B8F8B}">
       <formula1>$AV$9:$AV$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{EE551BFC-1380-4688-9CFB-83B42BA39880}">
-      <formula1>$AZ$9:$AZ$12</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{A6AF5BA9-5786-4E5D-9128-0DC2BA9560A5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{4FF43CEF-FECB-40EB-BEC3-FC4A0709E413}">
       <formula1>$AY$9:$AY$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{574AC30F-B080-4823-B035-087D318D4F00}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{ADEB3724-9972-4F22-86F6-A4B53CF65500}">
       <formula1>$AX$9:$AX$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{208E8586-A53E-49C9-8E44-9FD27DA62C5A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{1B6DA8E7-8921-46C2-B5F1-EDB330E8991D}">
       <formula1>$AW$9:$AW$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{488BC52E-41BD-40B5-A93D-07C549C24565}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 B10" xr:uid="{DB453DE4-A708-4192-8385-6ED22D70A9DA}">
       <formula1>$AU$9:$AU$12</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{6ABCC3A3-39D6-496C-BA51-98F3F4286434}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{8F8B861C-C393-4435-8DC0-EC8EEEE3BBFD}">
       <formula1>$AT$9:$AT$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{9A2FD3DB-3FAE-4601-8694-0155021F205A}">
+      <formula1>$BA$9:$BA$12</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{9168A5F5-CA80-4564-8DDA-57F03CF7364B}">
+      <formula1>$AZ$9:$AZ$10</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3486,9 +3560,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="str">
+      <c r="A1" s="1" t="e">
         <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B$9, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Completions Water Demand for Completions Sites over days [bbl/day]</v>
+        <v>#N/A</v>
       </c>
       <c r="H1" s="39"/>
     </row>
@@ -5377,7 +5451,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated decision period to match main in the operational case study
</commit_message>
<xml_diff>
--- a/pareto/case_studies/operational_generic_case_study.xlsx
+++ b/pareto/case_studies/operational_generic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naresh\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AB5981-F847-4E63-92CC-BB42B67223C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73318DC7-1BD4-442F-8E4C-F66330C958C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="770" firstSheet="1" activeTab="1" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="5685" yWindow="1785" windowWidth="28800" windowHeight="15375" tabRatio="770" firstSheet="1" activeTab="1" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -1816,15 +1816,15 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.21875" customWidth="1"/>
-    <col min="10" max="10" width="4.44140625" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="14"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -1836,7 +1836,7 @@
       <c r="J2" s="15"/>
       <c r="K2" s="16"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="17"/>
       <c r="C3" s="18" t="s">
         <v>10</v>
@@ -1850,7 +1850,7 @@
       <c r="J3" s="19"/>
       <c r="K3" s="20"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="17"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
@@ -1862,7 +1862,7 @@
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
       <c r="C5" s="19" t="s">
         <v>16</v>
@@ -1876,7 +1876,7 @@
       <c r="J5" s="19"/>
       <c r="K5" s="20"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="17"/>
       <c r="C6" s="19" t="s">
         <v>14</v>
@@ -1890,7 +1890,7 @@
       <c r="J6" s="19"/>
       <c r="K6" s="20"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="17"/>
       <c r="C7" s="19" t="s">
         <v>11</v>
@@ -1904,7 +1904,7 @@
       <c r="J7" s="19"/>
       <c r="K7" s="20"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="17"/>
       <c r="C8" s="19" t="s">
         <v>12</v>
@@ -1918,7 +1918,7 @@
       <c r="J8" s="19"/>
       <c r="K8" s="20"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="17"/>
       <c r="C9" s="19" t="s">
         <v>13</v>
@@ -1932,7 +1932,7 @@
       <c r="J9" s="19"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
       <c r="C10" s="19" t="s">
         <v>52</v>
@@ -1946,7 +1946,7 @@
       <c r="J10" s="19"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="17"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -1958,7 +1958,7 @@
       <c r="J11" s="19"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="17"/>
       <c r="C12" s="19" t="s">
         <v>17</v>
@@ -1972,7 +1972,7 @@
       <c r="J12" s="19"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="17"/>
       <c r="C13" s="19" t="s">
         <v>15</v>
@@ -1986,7 +1986,7 @@
       <c r="J13" s="19"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="17"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -1998,7 +1998,7 @@
       <c r="J14" s="19"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="17"/>
       <c r="C15" s="19" t="s">
         <v>18</v>
@@ -2012,7 +2012,7 @@
       <c r="J15" s="19"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="17"/>
       <c r="C16" s="19" t="s">
         <v>19</v>
@@ -2026,7 +2026,7 @@
       <c r="J16" s="19"/>
       <c r="K16" s="20"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="17"/>
       <c r="C17" s="19" t="s">
         <v>20</v>
@@ -2040,7 +2040,7 @@
       <c r="J17" s="19"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="17"/>
       <c r="C18" s="19" t="s">
         <v>21</v>
@@ -2054,7 +2054,7 @@
       <c r="J18" s="19"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="17"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -2066,7 +2066,7 @@
       <c r="J19" s="19"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="17"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
@@ -2078,7 +2078,7 @@
       <c r="J20" s="19"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="17"/>
       <c r="C21" s="21" t="s">
         <v>22</v>
@@ -2094,7 +2094,7 @@
       <c r="J21" s="19"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="17"/>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
@@ -2106,7 +2106,7 @@
       <c r="J22" s="19"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="17"/>
       <c r="C23" s="22" t="s">
         <v>24</v>
@@ -2122,7 +2122,7 @@
       <c r="J23" s="19"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="17"/>
       <c r="C24" s="22" t="s">
         <v>25</v>
@@ -2138,7 +2138,7 @@
       <c r="J24" s="19"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="17"/>
       <c r="C25" s="22" t="s">
         <v>26</v>
@@ -2154,7 +2154,7 @@
       <c r="J25" s="19"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="17"/>
       <c r="C26" s="22" t="s">
         <v>30</v>
@@ -2170,7 +2170,7 @@
       <c r="J26" s="19"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="17"/>
       <c r="C27" s="22" t="s">
         <v>32</v>
@@ -2186,7 +2186,7 @@
       <c r="J27" s="19"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="17"/>
       <c r="C28" s="22" t="s">
         <v>34</v>
@@ -2202,7 +2202,7 @@
       <c r="J28" s="19"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="17"/>
       <c r="C29" s="22" t="s">
         <v>35</v>
@@ -2218,7 +2218,7 @@
       <c r="J29" s="19"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="17"/>
       <c r="C30" s="22" t="s">
         <v>38</v>
@@ -2234,7 +2234,7 @@
       <c r="J30" s="19"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="17"/>
       <c r="C31" s="22" t="s">
         <v>40</v>
@@ -2253,7 +2253,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="17"/>
       <c r="C32" s="22" t="s">
         <v>43</v>
@@ -2269,7 +2269,7 @@
       <c r="J32" s="19"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="17"/>
       <c r="C33" s="22" t="s">
         <v>42</v>
@@ -2285,7 +2285,7 @@
       <c r="J33" s="19"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="17"/>
       <c r="C34" s="22" t="s">
         <v>46</v>
@@ -2301,7 +2301,7 @@
       <c r="J34" s="19"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="17"/>
       <c r="C35" s="22" t="s">
         <v>48</v>
@@ -2317,7 +2317,7 @@
       <c r="J35" s="19"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="17"/>
       <c r="C36" s="22" t="s">
         <v>49</v>
@@ -2333,7 +2333,7 @@
       <c r="J36" s="19"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="23"/>
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
@@ -2378,28 +2378,28 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.21875" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.21875" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.21875" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -2422,28 +2422,28 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.21875" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.21875" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.21875" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -2466,18 +2466,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>103</v>
       </c>
@@ -2488,7 +2488,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="27"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>104</v>
       </c>
@@ -2497,7 +2497,7 @@
       <c r="D3" s="9"/>
       <c r="E3" s="36"/>
     </row>
-    <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>105</v>
       </c>
@@ -2523,13 +2523,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>98</v>
       </c>
@@ -2546,7 +2546,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>75</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>76</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>2.083333333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
         <v>90</v>
       </c>
@@ -2583,12 +2583,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="40" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" s="40">
         <v>1</v>
       </c>
@@ -2611,9 +2611,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -2634,9 +2634,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -2657,13 +2657,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>93</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" s="39" t="s">
         <v>90</v>
       </c>
@@ -2742,17 +2742,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>98</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>75</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>76</v>
       </c>
@@ -2795,17 +2795,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>96</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -2838,18 +2838,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>93</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="C3" s="36"/>
     </row>
-    <row r="4" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -2921,37 +2921,37 @@
   <dimension ref="A1:BA12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="92.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="0.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="48" width="9.33203125" style="1"/>
-    <col min="49" max="49" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="92.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="0.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="48" width="9.28515625" style="1"/>
+    <col min="49" max="49" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:53" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>111</v>
       </c>
@@ -2971,7 +2971,7 @@
       <c r="J2" s="49"/>
       <c r="K2" s="51"/>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>115</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>122</v>
       </c>
@@ -3025,7 +3025,7 @@
       <c r="J4" s="56"/>
       <c r="K4" s="58"/>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>127</v>
       </c>
@@ -3043,7 +3043,7 @@
       <c r="J5" s="60"/>
       <c r="K5" s="61"/>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>130</v>
       </c>
@@ -3067,7 +3067,7 @@
       <c r="J6" s="60"/>
       <c r="K6" s="61"/>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>134</v>
       </c>
@@ -3091,7 +3091,7 @@
       <c r="J7" s="60"/>
       <c r="K7" s="61"/>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>139</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>154</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>159</v>
       </c>
@@ -3223,12 +3223,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
         <v>143</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D11" s="62" t="s">
         <v>145</v>
@@ -3259,7 +3259,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="AU12" s="1" t="s">
         <v>125</v>
       </c>
@@ -3310,17 +3310,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>96</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -3353,18 +3353,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>93</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
@@ -3434,7 +3434,7 @@
       <c r="N3" s="9"/>
       <c r="O3" s="36"/>
     </row>
-    <row r="4" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -3459,7 +3459,7 @@
       <c r="N4" s="9"/>
       <c r="O4" s="36"/>
     </row>
-    <row r="5" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -3486,7 +3486,7 @@
       <c r="N5" s="9"/>
       <c r="O5" s="36"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -3511,7 +3511,7 @@
       <c r="N6" s="9"/>
       <c r="O6" s="36"/>
     </row>
-    <row r="7" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -3552,21 +3552,21 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="9.21875" style="1"/>
+    <col min="1" max="7" width="9.28515625" style="1"/>
     <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.21875" style="1"/>
+    <col min="9" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="e">
         <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B$9, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>#N/A</v>
       </c>
       <c r="H1" s="39"/>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>96</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F8" s="12"/>
     </row>
   </sheetData>
@@ -3627,21 +3627,21 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="8" customWidth="1"/>
     <col min="2" max="2" width="23" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.21875" style="1"/>
+    <col min="3" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="str">
         <f>_xlfn.CONCAT( "Table of Production Rate Forecasts by Tanks and Pads"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Production Rate Forecasts by Tanks and Pads [bbl/day]</v>
       </c>
       <c r="B1" s="39"/>
     </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>93</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>4</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>4</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>4</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>5</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>5</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>5</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>6</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>6</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>6</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>7</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G21" s="12"/>
     </row>
   </sheetData>
@@ -4006,19 +4006,19 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" style="8" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="1" width="17.140625" style="8" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="str">
         <f>_xlfn.CONCAT( "Table of Production Rate Forecasts by Pads"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Production Rate Forecasts by Pads [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>93</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>1766</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F12" s="12"/>
     </row>
   </sheetData>
@@ -4158,19 +4158,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="8"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="1" width="9.28515625" style="8"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="str">
         <f>_xlfn.CONCAT( "Table of Flowback Rate Forecasts by Pads"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Flowback Rate Forecasts by Pads [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>96</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F8" s="12"/>
     </row>
   </sheetData>
@@ -4228,12 +4228,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Initial Disposal Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Initial Disposal Capacity [bbl/day]</v>
@@ -4241,7 +4241,7 @@
       <c r="B1" s="39"/>
       <c r="D1" s="39"/>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>97</v>
       </c>
@@ -4250,7 +4250,7 @@
       </c>
       <c r="D2" s="39"/>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>54</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>55</v>
       </c>
@@ -4267,7 +4267,7 @@
       </c>
       <c r="D4" s="39"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="39"/>
       <c r="B6" s="39"/>
       <c r="D6" s="39"/>
@@ -4287,9 +4287,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Table of Reuse Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Reuse Capacity [bbl/day]</v>
@@ -4309,19 +4309,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Availability"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Freshwater Sourcing Availability [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>98</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>75</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>76</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F9" s="12"/>
     </row>
   </sheetData>
@@ -4399,19 +4399,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="1" width="15.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Completions Pad Storage Capacity [bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>96</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4468,39 +4468,39 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="9.21875" style="1"/>
-    <col min="10" max="10" width="11.21875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="4.5546875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="9" width="9.28515625" style="1"/>
+    <col min="10" max="10" width="11.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="39"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="39"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -4508,12 +4508,12 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="39"/>
       <c r="C10" s="39"/>
     </row>
@@ -4533,19 +4533,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Pad Offloading Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Pad Offloading Capacity [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>96</v>
       </c>
@@ -4553,7 +4553,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4576,9 +4576,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Production Tank Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Production Tank Capacity [bbl]</v>
@@ -4600,18 +4600,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Disposal Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Disposal Operational Cost [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>97</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>54</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>55</v>
       </c>
@@ -4652,7 +4652,7 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4669,19 +4669,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Reuse Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Reuse Operational Cost [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>96</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4714,18 +4714,18 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Piping Operational Costs [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Piping Operational Costs [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>98</v>
       </c>
@@ -4733,7 +4733,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>75</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>76</v>
       </c>
@@ -4766,19 +4766,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Freshwater Sourcing Cost [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>98</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>75</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>76</v>
       </c>
@@ -4819,19 +4819,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity over Time [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Completions Pad Storage Capacity over Time [bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>96</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -4888,18 +4888,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Trucking Hourly Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", "hour","]")</f>
         <v>Table of Trucking Hourly Cost [USD/hour]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>94</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>8</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>75</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>76</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>3</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>4</v>
       </c>
@@ -4947,7 +4947,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>6</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33" t="s">
         <v>7</v>
       </c>
@@ -4988,20 +4988,20 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" style="1" customWidth="1"/>
-    <col min="2" max="6" width="9.21875" style="1"/>
-    <col min="7" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2" max="6" width="9.28515625" style="1"/>
+    <col min="7" max="8" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>101</v>
       </c>
@@ -5030,7 +5030,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -5047,7 +5047,7 @@
       </c>
       <c r="I3" s="36"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -5083,7 +5083,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -5134,7 +5134,7 @@
       </c>
       <c r="I8" s="36"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>75</v>
       </c>
@@ -5149,7 +5149,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="36"/>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>76</v>
       </c>
@@ -5164,7 +5164,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="36"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
@@ -5177,7 +5177,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="36"/>
     </row>
-    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>55</v>
       </c>
@@ -5190,7 +5190,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="11"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" s="13"/>
     </row>
   </sheetData>
@@ -5210,40 +5210,40 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.21875" style="1"/>
-    <col min="3" max="3" width="3.5546875" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.21875" style="1"/>
-    <col min="13" max="13" width="11.21875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5546875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="2" width="9.28515625" style="1"/>
+    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.28515625" style="1"/>
+    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D4" s="12"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>64</v>
       </c>
@@ -5251,52 +5251,52 @@
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>74</v>
       </c>
@@ -5319,17 +5319,17 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>103</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>104</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>105</v>
       </c>
@@ -5370,19 +5370,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Table of Water Quality of Produced Water and Flowback Water [",VLOOKUP("concentration", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Water Quality of Produced Water and Flowback Water [mg/liter]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>108</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
@@ -5398,7 +5398,7 @@
         <v>142277</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>140998</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>172490.2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -5422,7 +5422,7 @@
         <v>257547</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>7</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>241833.8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
@@ -5455,19 +5455,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Table of Initial Water Quality at Storage [",VLOOKUP("concentration", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Initial Water Quality at Storage [mg/liter]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>109</v>
       </c>
@@ -5475,7 +5475,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="45"/>
       <c r="B3" s="46"/>
     </row>
@@ -5496,30 +5496,30 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.21875" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.21875" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.21875" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
@@ -5542,28 +5542,28 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.21875" style="1"/>
-    <col min="4" max="4" width="4.44140625" style="1" customWidth="1"/>
-    <col min="5" max="14" width="9.21875" style="1"/>
-    <col min="15" max="15" width="12.109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.5546875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5" max="14" width="9.28515625" style="1"/>
+    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.5703125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>55</v>
       </c>
@@ -5586,30 +5586,30 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.21875" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.21875" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.21875" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>76</v>
       </c>
@@ -5635,28 +5635,28 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.21875" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.21875" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.21875" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -5679,30 +5679,30 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.21875" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.21875" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.21875" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>105</v>
       </c>

</xml_diff>

<commit_message>
correct missing flowback volumes under individual config options
</commit_message>
<xml_diff>
--- a/pareto/case_studies/operational_generic_case_study.xlsx
+++ b/pareto/case_studies/operational_generic_case_study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AC5AEE-63BA-4278-BFF3-85719F40EF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6B1DD6-AAE6-45BB-A03F-BD22F0B7CC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="770" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="770" firstSheet="12" activeTab="25" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -37,24 +37,25 @@
     <sheet name="CompletionsDemand" sheetId="8" r:id="rId22"/>
     <sheet name="ProductionRates" sheetId="40" r:id="rId23"/>
     <sheet name="PadRates" sheetId="56" r:id="rId24"/>
-    <sheet name="FlowbackRates" sheetId="58" r:id="rId25"/>
-    <sheet name="DisposalCapacity" sheetId="46" r:id="rId26"/>
-    <sheet name="TreatmentCapacity" sheetId="62" r:id="rId27"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId28"/>
-    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId29"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId30"/>
-    <sheet name="ProductionTankCapacity" sheetId="61" r:id="rId31"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId32"/>
-    <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId33"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId34"/>
-    <sheet name="PipelineOperationalCost" sheetId="54" r:id="rId35"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId36"/>
-    <sheet name="PadStorageCost" sheetId="70" r:id="rId37"/>
-    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId38"/>
-    <sheet name="TruckingTime" sheetId="7" r:id="rId39"/>
-    <sheet name="TreatmentEfficiency" sheetId="69" r:id="rId40"/>
-    <sheet name="PadWaterQuality" sheetId="71" r:id="rId41"/>
-    <sheet name="StorageInitialWaterQuality" sheetId="72" r:id="rId42"/>
+    <sheet name="TankFlowbackRates" sheetId="74" r:id="rId25"/>
+    <sheet name="FlowbackRates" sheetId="58" r:id="rId26"/>
+    <sheet name="DisposalCapacity" sheetId="46" r:id="rId27"/>
+    <sheet name="TreatmentCapacity" sheetId="62" r:id="rId28"/>
+    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId29"/>
+    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId30"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId31"/>
+    <sheet name="ProductionTankCapacity" sheetId="61" r:id="rId32"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId33"/>
+    <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId34"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId35"/>
+    <sheet name="PipelineOperationalCost" sheetId="54" r:id="rId36"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId37"/>
+    <sheet name="PadStorageCost" sheetId="70" r:id="rId38"/>
+    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId39"/>
+    <sheet name="TruckingTime" sheetId="7" r:id="rId40"/>
+    <sheet name="TreatmentEfficiency" sheetId="69" r:id="rId41"/>
+    <sheet name="PadWaterQuality" sheetId="71" r:id="rId42"/>
+    <sheet name="StorageInitialWaterQuality" sheetId="72" r:id="rId43"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -74,8 +75,172 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Andres Calderon</author>
+  </authors>
+  <commentList>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{99618F5E-9634-421E-A41A-271BAE2797D1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Andres Calderon:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This value is added as "clutter" for testing purposes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{DAF72A8D-E948-4544-A79F-2A2DB092DF89}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Andres Calderon:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Contains white spaces for testing purposes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{B3BE548B-9451-4ACE-845C-1C70635761A5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Andres Calderon:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cell with some calculations for testing purposes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{D5A71132-39A3-4638-9D45-CAE15CC160EB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Andres Calderon:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Contains white spaces for testing purposes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{875F4A7E-B8F1-4274-9617-5F7FC3688FD8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Andres Calderon:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This value is added as "clutter" for testing purposes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Andres Calderon</author>
+  </authors>
+  <commentList>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{D285F83C-4D6A-4221-AB67-25E4DE633D02}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Andres Calderon:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This cell used to contain data that was deleted. This was a common source of errors when using get_data()</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="163">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -347,6 +512,12 @@
     <t>Production Pads to Treatment Facilities Trucking Arcs [-]</t>
   </si>
   <si>
+    <t>PROPRIETARY DATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
     <t xml:space="preserve">    </t>
   </si>
   <si>
@@ -531,6 +702,33 @@
   </si>
   <si>
     <t>meter</t>
+  </si>
+  <si>
+    <t>pressure</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>Pressure units when using the hydraulics module</t>
+  </si>
+  <si>
+    <t>6895 Pa</t>
+  </si>
+  <si>
+    <t>pascal</t>
+  </si>
+  <si>
+    <t>elevation</t>
+  </si>
+  <si>
+    <t>Elevation of a network node (including all sites)</t>
+  </si>
+  <si>
+    <t>B01</t>
+  </si>
+  <si>
+    <t>B02</t>
   </si>
 </sst>
 </file>
@@ -540,7 +738,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -607,6 +805,19 @@
       <family val="1"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -614,7 +825,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,6 +841,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1069,9 +1286,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1150,6 +1367,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1168,54 +1386,54 @@
     <xf numFmtId="43" fontId="3" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="3" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1227,6 +1445,7 @@
     <xf numFmtId="43" fontId="1" fillId="3" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1603,11 +1822,11 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.21875" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" customWidth="1"/>
     <col min="10" max="10" width="4.44140625" customWidth="1"/>
     <col min="11" max="11" width="9.44140625" customWidth="1"/>
   </cols>
@@ -2167,17 +2386,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.21875" style="1"/>
+    <col min="1" max="3" width="9.33203125" style="1"/>
     <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.21875" style="1"/>
+    <col min="6" max="13" width="9.33203125" style="1"/>
     <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.21875" style="1"/>
+    <col min="18" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -2211,17 +2430,17 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.21875" style="1"/>
+    <col min="1" max="3" width="9.33203125" style="1"/>
     <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.21875" style="1"/>
+    <col min="6" max="13" width="9.33203125" style="1"/>
     <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.21875" style="1"/>
+    <col min="18" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -2252,7 +2471,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2263,31 +2482,37 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="36"/>
+        <v>104</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>105</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2296,39 +2521,38 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="39"/>
+      <c r="B1" s="39" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -2337,8 +2561,11 @@
       <c r="B3" s="36">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>90</v>
+      <c r="E3" s="40">
+        <v>1</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2348,14 +2575,36 @@
       <c r="B4" s="11">
         <v>1</v>
       </c>
+      <c r="D4" s="40">
+        <f>1+1/2+1/3+1/4</f>
+        <v>2.083333333333333</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="39"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D8" s="40">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2413,24 +2662,26 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="39"/>
+      <c r="E1" s="39" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -2477,7 +2728,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D9" s="39"/>
+      <c r="D9" s="39" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2487,19 +2740,19 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED7A596-FF30-4282-98C8-7AB378F1FE03}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED7A596-FF30-4282-98C8-7AB378F1FE03}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2509,7 +2762,7 @@
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -2530,11 +2783,12 @@
       <c r="B4" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2549,9 +2803,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2561,7 +2815,7 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -2592,10 +2846,10 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.88671875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2605,7 +2859,7 @@
     </row>
     <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>54</v>
@@ -2672,9 +2926,11 @@
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
   </sheetPr>
-  <dimension ref="A1:AZ12"/>
+  <dimension ref="A1:BA12"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2693,306 +2949,357 @@
     <col min="49" max="49" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="16384" width="9.33203125" style="1"/>
+    <col min="52" max="52" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:52" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:53" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="50"/>
-    </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="D2" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="51"/>
+    </row>
+    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="E3" s="53" t="s">
-        <v>114</v>
-      </c>
-      <c r="F3" s="54" t="s">
+      <c r="B3" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="55" t="s">
+      <c r="D3" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="H3" s="56"/>
-      <c r="I3" s="55" t="s">
+      <c r="E3" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="G3" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" s="57"/>
+      <c r="I3" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="K3" s="58" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="54" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="57"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="58"/>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="59"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="61"/>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" s="53"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="61"/>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>138</v>
+      </c>
+      <c r="H7" s="53"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="61"/>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="61"/>
+      <c r="AT8" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="AU8" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="AV8" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW8" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="AX8" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="AY8" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="AZ8" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="BA8" s="37" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="53" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="59" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="G9" s="60" t="s">
+        <v>157</v>
+      </c>
+      <c r="H9" s="53"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="61"/>
+      <c r="AT9" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="K3" s="57" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
+      <c r="AU9" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AV9" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AW9" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AX9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AY9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AZ9" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="BA9" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" s="59"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="61"/>
+      <c r="AT10" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="51" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" s="52" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" s="53" t="s">
+      <c r="AU10" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F4" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="G4" s="55" t="s">
-        <v>124</v>
-      </c>
-      <c r="H4" s="56"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="57"/>
-    </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
+      <c r="AV10" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AW10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AX10" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY10" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AZ10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="BA10" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="D11" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="G11" s="65" t="s">
+        <v>147</v>
+      </c>
+      <c r="H11" s="62"/>
+      <c r="I11" s="66" t="s">
+        <v>148</v>
+      </c>
+      <c r="J11" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="K11" s="65" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU11" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="BA11" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AU12" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B5" s="51" t="s">
-        <v>126</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" s="58"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="60"/>
-    </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="51" t="s">
-        <v>129</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="53" t="s">
-        <v>129</v>
-      </c>
-      <c r="F6" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="G6" s="55" t="s">
-        <v>131</v>
-      </c>
-      <c r="H6" s="52"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="60"/>
-    </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="D7" s="52" t="s">
-        <v>134</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>135</v>
-      </c>
-      <c r="F7" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="G7" s="55" t="s">
-        <v>136</v>
-      </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="60"/>
-    </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="51" t="s">
-        <v>138</v>
-      </c>
-      <c r="D8" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="E8" s="58"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="60"/>
-      <c r="AT8" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="AU8" s="37" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV8" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="AW8" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="AX8" s="37" t="s">
-        <v>132</v>
-      </c>
-      <c r="AY8" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="AZ8" s="37" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:52" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>138</v>
-      </c>
-      <c r="D9" s="61" t="s">
-        <v>143</v>
-      </c>
-      <c r="E9" s="62" t="s">
-        <v>144</v>
-      </c>
-      <c r="F9" s="63" t="s">
-        <v>116</v>
-      </c>
-      <c r="G9" s="64" t="s">
-        <v>145</v>
-      </c>
-      <c r="H9" s="61"/>
-      <c r="I9" s="65" t="s">
-        <v>146</v>
-      </c>
-      <c r="J9" s="63" t="s">
-        <v>116</v>
-      </c>
-      <c r="K9" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="AT9" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="AU9" s="1" t="s">
+      <c r="BA12" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="AV9" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AW9" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="AX9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AY9" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="AZ9" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="AT10" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AU10" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="AV10" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AW10" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AX10" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="AY10" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AZ10" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="AU11" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AZ11" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="AU12" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="AZ12" s="1" t="s">
-        <v>146</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{983EC2A0-C4EA-4CE0-BED1-203B514C4F46}">
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{86102F73-0552-4E90-BC6E-A014997B8F8B}">
       <formula1>$AV$9:$AV$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{EE551BFC-1380-4688-9CFB-83B42BA39880}">
-      <formula1>$AZ$9:$AZ$12</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{A6AF5BA9-5786-4E5D-9128-0DC2BA9560A5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{4FF43CEF-FECB-40EB-BEC3-FC4A0709E413}">
       <formula1>$AY$9:$AY$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{574AC30F-B080-4823-B035-087D318D4F00}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{ADEB3724-9972-4F22-86F6-A4B53CF65500}">
       <formula1>$AX$9:$AX$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{208E8586-A53E-49C9-8E44-9FD27DA62C5A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{1B6DA8E7-8921-46C2-B5F1-EDB330E8991D}">
       <formula1>$AW$9:$AW$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{488BC52E-41BD-40B5-A93D-07C549C24565}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 B10" xr:uid="{DB453DE4-A708-4192-8385-6ED22D70A9DA}">
       <formula1>$AU$9:$AU$12</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{6ABCC3A3-39D6-496C-BA51-98F3F4286434}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{8F8B861C-C393-4435-8DC0-EC8EEEE3BBFD}">
       <formula1>$AT$9:$AT$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{9A2FD3DB-3FAE-4601-8694-0155021F205A}">
+      <formula1>$BA$9:$BA$12</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{9168A5F5-CA80-4564-8DDA-57F03CF7364B}">
+      <formula1>$AZ$9:$AZ$10</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3011,9 +3318,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3023,7 +3330,7 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>54</v>
@@ -3048,26 +3355,26 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>61</v>
@@ -3111,8 +3418,14 @@
       <c r="O2" s="27" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P2" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
@@ -3134,8 +3447,10 @@
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
       <c r="O3" s="36"/>
-    </row>
-    <row r="4" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P3" s="9"/>
+      <c r="Q3" s="36"/>
+    </row>
+    <row r="4" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -3159,8 +3474,10 @@
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
       <c r="O4" s="36"/>
-    </row>
-    <row r="5" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P4" s="9"/>
+      <c r="Q4" s="36"/>
+    </row>
+    <row r="5" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -3186,8 +3503,10 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
       <c r="O5" s="36"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5" s="9"/>
+      <c r="Q5" s="36"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -3211,8 +3530,10 @@
       </c>
       <c r="N6" s="9"/>
       <c r="O6" s="36"/>
-    </row>
-    <row r="7" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P6" s="9"/>
+      <c r="Q6" s="36"/>
+    </row>
+    <row r="7" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -3232,6 +3553,33 @@
         <v>1</v>
       </c>
       <c r="O7" s="11">
+        <v>1</v>
+      </c>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3253,23 +3601,23 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="9.21875" style="1"/>
+    <col min="1" max="7" width="9.33203125" style="1"/>
     <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.21875" style="1"/>
+    <col min="9" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B$9, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B11, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
         <v>Table of Completions Water Demand for Completions Sites over days [bbl/day]</v>
       </c>
       <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
@@ -3325,14 +3673,14 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.109375" style="8" customWidth="1"/>
     <col min="2" max="2" width="23" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.21875" style="1"/>
+    <col min="3" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3344,10 +3692,10 @@
     </row>
     <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>56</v>
@@ -3707,10 +4055,10 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" style="8" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3721,7 +4069,7 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
@@ -3849,70 +4197,101 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16A47F7-A2FF-4DEE-B278-2DA8AB93D602}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1F3225-05BE-4B0D-AE83-9F04DDDFE920}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="8"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="8" width="9.33203125" style="1"/>
+    <col min="9" max="9" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="str">
-        <f>_xlfn.CONCAT( "Table of Flowback Rate Forecasts by Pads"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Flowback Rate Forecasts by Pads [bbl/day]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B11, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
+        <v>Table of Completions Water Demand for Completions Sites over days [bbl/day]</v>
+      </c>
+      <c r="I1" s="39"/>
+    </row>
+    <row r="2" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="G2" s="27" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="33" t="s">
+    <row r="3" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="10">
-        <v>500</v>
+      <c r="B3" s="70" t="s">
+        <v>161</v>
       </c>
       <c r="C3" s="10">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="D3" s="10">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="E3" s="10">
-        <v>500</v>
-      </c>
-      <c r="F3" s="11">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F8" s="12"/>
+        <v>250</v>
+      </c>
+      <c r="F3" s="10">
+        <v>250</v>
+      </c>
+      <c r="G3" s="10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="70" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="10">
+        <v>250</v>
+      </c>
+      <c r="D4" s="10">
+        <v>250</v>
+      </c>
+      <c r="E4" s="10">
+        <v>250</v>
+      </c>
+      <c r="F4" s="10">
+        <v>250</v>
+      </c>
+      <c r="G4" s="10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G8" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3921,6 +4300,78 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16A47F7-A2FF-4DEE-B278-2DA8AB93D602}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" style="8"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="str">
+        <f>_xlfn.CONCAT( "Table of Flowback Rate Forecasts by Pads"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Flowback Rate Forecasts by Pads [bbl/day]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10">
+        <v>500</v>
+      </c>
+      <c r="C3" s="10">
+        <v>500</v>
+      </c>
+      <c r="D3" s="10">
+        <v>500</v>
+      </c>
+      <c r="E3" s="10">
+        <v>500</v>
+      </c>
+      <c r="F3" s="11">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -3929,9 +4380,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3944,10 +4395,10 @@
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D2" s="39"/>
     </row>
@@ -3979,7 +4430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59865970-D83F-46CB-8781-62CE35DBF4B5}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4001,7 +4452,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4010,10 +4461,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4024,7 +4475,7 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
@@ -4084,73 +4535,6 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F9" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA48CF8D-5373-4539-A55F-3258FEB20DFB}">
-  <sheetPr>
-    <tabColor rgb="FFD9C6FE"/>
-  </sheetPr>
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Completions Pad Storage Capacity [bbl]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="41">
-        <v>10000</v>
-      </c>
-      <c r="C3" s="41">
-        <v>10000</v>
-      </c>
-      <c r="D3" s="41">
-        <v>10000</v>
-      </c>
-      <c r="E3" s="41">
-        <v>10000</v>
-      </c>
-      <c r="F3" s="42">
-        <v>10000</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4169,14 +4553,14 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="9.21875" style="1"/>
-    <col min="10" max="10" width="11.21875" style="1" customWidth="1"/>
+    <col min="1" max="9" width="9.33203125" style="1"/>
+    <col min="10" max="10" width="11.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="10.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="12.88671875" style="1" customWidth="1"/>
     <col min="13" max="13" width="4.5546875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.21875" style="1"/>
+    <col min="14" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -4226,6 +4610,73 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA48CF8D-5373-4539-A55F-3258FEB20DFB}">
+  <sheetPr>
+    <tabColor rgb="FFD9C6FE"/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Completions Pad Storage Capacity [bbl]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="42">
+        <v>10000</v>
+      </c>
+      <c r="C3" s="42">
+        <v>10000</v>
+      </c>
+      <c r="D3" s="42">
+        <v>10000</v>
+      </c>
+      <c r="E3" s="42">
+        <v>10000</v>
+      </c>
+      <c r="F3" s="43">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4234,10 +4685,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4248,10 +4699,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4268,7 +4719,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EB27A2-91E8-4B14-8B2B-D8903B8CA8E8}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4290,7 +4741,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4301,9 +4752,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4314,10 +4765,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4342,7 +4793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74013BD9-1426-4BFB-8D02-5A2A33597048}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4359,7 +4810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4370,10 +4821,10 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.88671875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4384,10 +4835,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4404,7 +4855,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FF3D68-9420-4DF5-8A14-DD803657C7A5}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4415,9 +4866,9 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4428,7 +4879,7 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -4456,7 +4907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4467,10 +4918,10 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4481,10 +4932,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4509,7 +4960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2915391D-1D4E-446C-B6C1-F25D75A5D98F}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4534,9 +4985,9 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>56</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -4556,19 +5007,19 @@
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="41">
+      <c r="B3" s="42">
         <v>250</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="42">
         <v>250</v>
       </c>
-      <c r="D3" s="41">
+      <c r="D3" s="42">
         <v>250</v>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="42">
         <v>250</v>
       </c>
-      <c r="F3" s="42">
+      <c r="F3" s="43">
         <v>250</v>
       </c>
     </row>
@@ -4578,7 +5029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4589,9 +5040,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4602,10 +5053,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4671,228 +5122,6 @@
       <c r="B10" s="11">
         <v>92</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:I17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.77734375" style="1" customWidth="1"/>
-    <col min="2" max="6" width="9.21875" style="1"/>
-    <col min="7" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9">
-        <v>1</v>
-      </c>
-      <c r="H3" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="I3" s="36"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="H4" s="9">
-        <v>1</v>
-      </c>
-      <c r="I4" s="36">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9">
-        <v>2</v>
-      </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="36">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="36">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9">
-        <v>3</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9">
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="H8" s="9">
-        <v>2</v>
-      </c>
-      <c r="I8" s="36"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9">
-        <v>2</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="36"/>
-    </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="36"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="36"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="11"/>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G17" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4905,22 +5134,22 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.21875" style="1"/>
+    <col min="1" max="2" width="9.33203125" style="1"/>
     <col min="3" max="3" width="3.5546875" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.21875" style="1"/>
-    <col min="13" max="13" width="11.21875" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.33203125" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="10.6640625" style="1" customWidth="1"/>
     <col min="15" max="15" width="12.88671875" style="1" customWidth="1"/>
     <col min="16" max="16" width="4.5546875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.21875" style="1"/>
+    <col min="17" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -5000,6 +5229,16 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -5010,6 +5249,228 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2" max="6" width="9.33203125" style="1"/>
+    <col min="7" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.33203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="I3" s="36"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="H4" s="9">
+        <v>1</v>
+      </c>
+      <c r="I4" s="36">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9">
+        <v>2</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="36">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9">
+        <v>3</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="H8" s="9">
+        <v>2</v>
+      </c>
+      <c r="I8" s="36"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9">
+        <v>2</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="36"/>
+    </row>
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="36"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="36"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G17" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4E39D9-E2B5-4E92-A460-6BB588CED0C5}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -5027,20 +5488,20 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B3" s="36">
         <v>1</v>
@@ -5048,7 +5509,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
@@ -5060,7 +5521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3E2031-E70C-46E6-B55F-07206AFEE600}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -5085,17 +5546,17 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>105</v>
+        <v>108</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="66">
+      <c r="B3" s="67">
         <v>142277</v>
       </c>
     </row>
@@ -5103,7 +5564,7 @@
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="67">
+      <c r="B4" s="68">
         <v>140998</v>
       </c>
     </row>
@@ -5111,7 +5572,7 @@
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="67">
+      <c r="B5" s="68">
         <v>172490.2</v>
       </c>
     </row>
@@ -5119,7 +5580,7 @@
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="67">
+      <c r="B6" s="68">
         <v>257547</v>
       </c>
     </row>
@@ -5127,7 +5588,7 @@
       <c r="A7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="67">
+      <c r="B7" s="68">
         <v>241833.8</v>
       </c>
     </row>
@@ -5135,7 +5596,7 @@
       <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="68">
+      <c r="B8" s="69">
         <v>188503.7</v>
       </c>
     </row>
@@ -5145,7 +5606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465369F7-E9A8-4A2B-BBBA-6F1C07C7C51F}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -5170,15 +5631,15 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="43" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="44"/>
-      <c r="B3" s="45"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="46"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5197,17 +5658,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.21875" style="1"/>
+    <col min="1" max="3" width="9.33203125" style="1"/>
     <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.21875" style="1"/>
+    <col min="6" max="13" width="9.33203125" style="1"/>
     <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.21875" style="1"/>
+    <col min="18" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -5243,15 +5704,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.21875" style="1"/>
+    <col min="1" max="3" width="9.33203125" style="1"/>
     <col min="4" max="4" width="4.44140625" style="1" customWidth="1"/>
-    <col min="5" max="14" width="9.21875" style="1"/>
+    <col min="5" max="14" width="9.33203125" style="1"/>
     <col min="15" max="15" width="12.109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="4.5546875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.21875" style="1"/>
+    <col min="18" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -5287,17 +5748,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.21875" style="1"/>
+    <col min="1" max="3" width="9.33203125" style="1"/>
     <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.21875" style="1"/>
+    <col min="6" max="13" width="9.33203125" style="1"/>
     <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.21875" style="1"/>
+    <col min="18" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -5336,17 +5797,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.21875" style="1"/>
+    <col min="1" max="3" width="9.33203125" style="1"/>
     <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.21875" style="1"/>
+    <col min="6" max="13" width="9.33203125" style="1"/>
     <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.21875" style="1"/>
+    <col min="18" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -5380,17 +5841,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.21875" style="1"/>
+    <col min="1" max="3" width="9.33203125" style="1"/>
     <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.21875" style="1"/>
+    <col min="6" max="13" width="9.33203125" style="1"/>
     <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.21875" style="1"/>
+    <col min="18" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -5400,12 +5861,12 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>

</xml_diff>

<commit_message>
re-remove operational input testing cells (highlights, comments, etc)
</commit_message>
<xml_diff>
--- a/pareto/case_studies/operational_generic_case_study.xlsx
+++ b/pareto/case_studies/operational_generic_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6B1DD6-AAE6-45BB-A03F-BD22F0B7CC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E48321-923B-48F5-8BE6-3E12B24E4753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="770" firstSheet="12" activeTab="25" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="770" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -75,172 +75,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Andres Calderon</author>
-  </authors>
-  <commentList>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{99618F5E-9634-421E-A41A-271BAE2797D1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This value is added as "clutter" for testing purposes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{DAF72A8D-E948-4544-A79F-2A2DB092DF89}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Contains white spaces for testing purposes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{B3BE548B-9451-4ACE-845C-1C70635761A5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Cell with some calculations for testing purposes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{D5A71132-39A3-4638-9D45-CAE15CC160EB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Contains white spaces for testing purposes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{875F4A7E-B8F1-4274-9617-5F7FC3688FD8}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This value is added as "clutter" for testing purposes</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Andres Calderon</author>
-  </authors>
-  <commentList>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{D285F83C-4D6A-4221-AB67-25E4DE633D02}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This cell used to contain data that was deleted. This was a common source of errors when using get_data()</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="161">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -510,12 +346,6 @@
   </si>
   <si>
     <t>Production Pads to Treatment Facilities Trucking Arcs [-]</t>
-  </si>
-  <si>
-    <t>PROPRIETARY DATA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     </t>
   </si>
   <si>
     <t xml:space="preserve">    </t>
@@ -738,7 +568,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -805,19 +635,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -825,7 +642,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -841,12 +658,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1286,9 +1097,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1367,7 +1178,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1386,54 +1196,54 @@
     <xf numFmtId="43" fontId="3" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="3" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1822,7 +1632,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2482,12 +2292,12 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>8</v>
@@ -2498,7 +2308,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -2507,7 +2317,7 @@
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -2521,14 +2331,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2541,18 +2351,18 @@
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="39" t="s">
-        <v>90</v>
-      </c>
+      <c r="B1" s="39"/>
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -2561,11 +2371,8 @@
       <c r="B3" s="36">
         <v>1</v>
       </c>
-      <c r="E3" s="40">
-        <v>1</v>
-      </c>
-      <c r="F3" s="40" t="s">
-        <v>92</v>
+      <c r="F3" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2575,36 +2382,10 @@
       <c r="B4" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="40">
-        <f>1+1/2+1/3+1/4</f>
-        <v>2.083333333333333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D8" s="40">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2662,7 +2443,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2675,13 +2456,11 @@
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="39" t="s">
-        <v>90</v>
-      </c>
+      <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -2728,9 +2507,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D9" s="39" t="s">
-        <v>90</v>
-      </c>
+      <c r="D9" s="39"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2740,14 +2517,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED7A596-FF30-4282-98C8-7AB378F1FE03}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED7A596-FF30-4282-98C8-7AB378F1FE03}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2755,20 +2532,20 @@
     <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>75</v>
       </c>
@@ -2776,19 +2553,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
         <v>76</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2815,7 +2590,7 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -2859,7 +2634,7 @@
     </row>
     <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>54</v>
@@ -2956,323 +2731,323 @@
   <sheetData>
     <row r="1" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:53" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="E2" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="51"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="50"/>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="E3" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="G3" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="H3" s="56"/>
+      <c r="I3" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="F3" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="G3" s="56" t="s">
+      <c r="K3" s="57" t="s">
         <v>119</v>
-      </c>
-      <c r="H3" s="57"/>
-      <c r="I3" s="56" t="s">
-        <v>120</v>
-      </c>
-      <c r="J3" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="K3" s="58" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="52" t="s">
         <v>122</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="E4" s="53" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="F4" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="E4" s="54" t="s">
-        <v>125</v>
-      </c>
-      <c r="F4" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="G4" s="56" t="s">
-        <v>126</v>
-      </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="58"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="57"/>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="52" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="53" t="s">
-        <v>129</v>
-      </c>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="61"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="60"/>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="E6" s="53" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="53" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="54" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="G6" s="56" t="s">
-        <v>133</v>
-      </c>
-      <c r="H6" s="53"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="61"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="60"/>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="E7" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="F7" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="55" t="s">
         <v>136</v>
       </c>
-      <c r="E7" s="54" t="s">
-        <v>137</v>
-      </c>
-      <c r="F7" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="G7" s="56" t="s">
-        <v>138</v>
-      </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="61"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="60"/>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="52" t="s">
         <v>139</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="E8" s="58"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="60"/>
+      <c r="AT8" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="AU8" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV8" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="AW8" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="AX8" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="AY8" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ8" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="BA8" s="37" t="s">
         <v>140</v>
-      </c>
-      <c r="D8" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="61"/>
-      <c r="AT8" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="AU8" s="37" t="s">
-        <v>122</v>
-      </c>
-      <c r="AV8" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW8" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="AX8" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="AY8" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="AZ8" s="37" t="s">
-        <v>154</v>
-      </c>
-      <c r="BA8" s="37" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="E9" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="F9" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="G9" s="59" t="s">
         <v>155</v>
       </c>
-      <c r="D9" s="53" t="s">
+      <c r="H9" s="52"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="60"/>
+      <c r="AT9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AU9" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AV9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW9" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AX9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AY9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AZ9" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E9" s="59" t="s">
-        <v>155</v>
-      </c>
-      <c r="F9" s="60" t="s">
-        <v>118</v>
-      </c>
-      <c r="G9" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="H9" s="53"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="61"/>
-      <c r="AT9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AU9" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AV9" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AW9" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="AX9" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="AY9" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="AZ9" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="BA9" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="B10" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" s="58"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="60"/>
+      <c r="AT10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AU10" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AV10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AW10" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="D10" s="53" t="s">
-        <v>160</v>
-      </c>
-      <c r="E10" s="59"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="61"/>
-      <c r="AT10" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="AV10" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AW10" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="AX10" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AY10" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AZ10" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="BA10" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="61" t="s">
         <v>143</v>
       </c>
-      <c r="B11" s="43" t="s">
-        <v>140</v>
-      </c>
-      <c r="D11" s="62" t="s">
+      <c r="E11" s="62" t="s">
+        <v>144</v>
+      </c>
+      <c r="F11" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="G11" s="64" t="s">
         <v>145</v>
       </c>
-      <c r="E11" s="63" t="s">
+      <c r="H11" s="61"/>
+      <c r="I11" s="65" t="s">
         <v>146</v>
       </c>
-      <c r="F11" s="64" t="s">
-        <v>118</v>
-      </c>
-      <c r="G11" s="65" t="s">
+      <c r="J11" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="K11" s="64" t="s">
         <v>147</v>
       </c>
-      <c r="H11" s="62"/>
-      <c r="I11" s="66" t="s">
-        <v>148</v>
-      </c>
-      <c r="J11" s="64" t="s">
-        <v>118</v>
-      </c>
-      <c r="K11" s="65" t="s">
-        <v>149</v>
-      </c>
       <c r="AU11" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="BA11" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.3">
       <c r="AU12" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="BA12" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -3330,7 +3105,7 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>54</v>
@@ -3374,7 +3149,7 @@
     </row>
     <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>61</v>
@@ -3419,10 +3194,10 @@
         <v>74</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="Q2" s="27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -3617,7 +3392,7 @@
     </row>
     <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
@@ -3692,10 +3467,10 @@
     </row>
     <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>93</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>95</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>56</v>
@@ -4069,7 +3844,7 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
@@ -4223,10 +3998,10 @@
     </row>
     <row r="2" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>56</v>
@@ -4248,8 +4023,8 @@
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="70" t="s">
-        <v>161</v>
+      <c r="B3" s="69" t="s">
+        <v>159</v>
       </c>
       <c r="C3" s="10">
         <v>250</v>
@@ -4271,8 +4046,8 @@
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="70" t="s">
-        <v>162</v>
+      <c r="B4" s="69" t="s">
+        <v>160</v>
       </c>
       <c r="C4" s="10">
         <v>250</v>
@@ -4306,7 +4081,7 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4324,7 +4099,7 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
@@ -4395,10 +4170,10 @@
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D2" s="39"/>
     </row>
@@ -4475,7 +4250,7 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
@@ -4632,9 +4407,9 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="40" t="s">
         <v>56</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -4654,19 +4429,19 @@
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3" s="41">
         <v>10000</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="41">
         <v>10000</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="41">
         <v>10000</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="41">
         <v>10000</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="42">
         <v>10000</v>
       </c>
     </row>
@@ -4699,10 +4474,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4765,10 +4540,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4835,10 +4610,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4879,7 +4654,7 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -4932,10 +4707,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4985,9 +4760,9 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="40" t="s">
         <v>56</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -5007,19 +4782,19 @@
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3" s="41">
         <v>250</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="41">
         <v>250</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="41">
         <v>250</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="41">
         <v>250</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="42">
         <v>250</v>
       </c>
     </row>
@@ -5053,10 +4828,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5233,12 +5008,12 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -5274,7 +5049,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>3</v>
@@ -5488,20 +5263,20 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="36">
         <v>1</v>
@@ -5509,7 +5284,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
@@ -5546,17 +5321,17 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="67">
+      <c r="B3" s="66">
         <v>142277</v>
       </c>
     </row>
@@ -5564,7 +5339,7 @@
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="68">
+      <c r="B4" s="67">
         <v>140998</v>
       </c>
     </row>
@@ -5572,7 +5347,7 @@
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="68">
+      <c r="B5" s="67">
         <v>172490.2</v>
       </c>
     </row>
@@ -5580,7 +5355,7 @@
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="68">
+      <c r="B6" s="67">
         <v>257547</v>
       </c>
     </row>
@@ -5588,7 +5363,7 @@
       <c r="A7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="68">
+      <c r="B7" s="67">
         <v>241833.8</v>
       </c>
     </row>
@@ -5596,7 +5371,7 @@
       <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="69">
+      <c r="B8" s="68">
         <v>188503.7</v>
       </c>
     </row>
@@ -5631,15 +5406,15 @@
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="44" t="s">
         <v>107</v>
       </c>
+      <c r="B2" s="43" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5861,12 +5636,12 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>

</xml_diff>

<commit_message>
merge conflicts with operational case study file and run black for jupyter notebooks
</commit_message>
<xml_diff>
--- a/pareto/case_studies/operational_generic_case_study.xlsx
+++ b/pareto/case_studies/operational_generic_case_study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naresh\project-pareto\pareto\case_studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73318DC7-1BD4-442F-8E4C-F66330C958C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E48321-923B-48F5-8BE6-3E12B24E4753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5685" yWindow="1785" windowWidth="28800" windowHeight="15375" tabRatio="770" firstSheet="1" activeTab="1" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="770" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -37,24 +37,25 @@
     <sheet name="CompletionsDemand" sheetId="8" r:id="rId22"/>
     <sheet name="ProductionRates" sheetId="40" r:id="rId23"/>
     <sheet name="PadRates" sheetId="56" r:id="rId24"/>
-    <sheet name="FlowbackRates" sheetId="58" r:id="rId25"/>
-    <sheet name="DisposalCapacity" sheetId="46" r:id="rId26"/>
-    <sheet name="TreatmentCapacity" sheetId="62" r:id="rId27"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId28"/>
-    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId29"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId30"/>
-    <sheet name="ProductionTankCapacity" sheetId="61" r:id="rId31"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId32"/>
-    <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId33"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId34"/>
-    <sheet name="PipelineOperationalCost" sheetId="54" r:id="rId35"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId36"/>
-    <sheet name="PadStorageCost" sheetId="70" r:id="rId37"/>
-    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId38"/>
-    <sheet name="TruckingTime" sheetId="7" r:id="rId39"/>
-    <sheet name="TreatmentEfficiency" sheetId="69" r:id="rId40"/>
-    <sheet name="PadWaterQuality" sheetId="71" r:id="rId41"/>
-    <sheet name="StorageInitialWaterQuality" sheetId="72" r:id="rId42"/>
+    <sheet name="TankFlowbackRates" sheetId="74" r:id="rId25"/>
+    <sheet name="FlowbackRates" sheetId="58" r:id="rId26"/>
+    <sheet name="DisposalCapacity" sheetId="46" r:id="rId27"/>
+    <sheet name="TreatmentCapacity" sheetId="62" r:id="rId28"/>
+    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId29"/>
+    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId30"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId31"/>
+    <sheet name="ProductionTankCapacity" sheetId="61" r:id="rId32"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId33"/>
+    <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId34"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId35"/>
+    <sheet name="PipelineOperationalCost" sheetId="54" r:id="rId36"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId37"/>
+    <sheet name="PadStorageCost" sheetId="70" r:id="rId38"/>
+    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId39"/>
+    <sheet name="TruckingTime" sheetId="7" r:id="rId40"/>
+    <sheet name="TreatmentEfficiency" sheetId="69" r:id="rId41"/>
+    <sheet name="PadWaterQuality" sheetId="71" r:id="rId42"/>
+    <sheet name="StorageInitialWaterQuality" sheetId="72" r:id="rId43"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -74,172 +75,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Andres Calderon</author>
-  </authors>
-  <commentList>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{99618F5E-9634-421E-A41A-271BAE2797D1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This value is added as "clutter" for testing purposes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{DAF72A8D-E948-4544-A79F-2A2DB092DF89}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Contains white spaces for testing purposes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{B3BE548B-9451-4ACE-845C-1C70635761A5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Cell with some calculations for testing purposes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{D5A71132-39A3-4638-9D45-CAE15CC160EB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Contains white spaces for testing purposes</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{875F4A7E-B8F1-4274-9617-5F7FC3688FD8}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This value is added as "clutter" for testing purposes</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Andres Calderon</author>
-  </authors>
-  <commentList>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{D285F83C-4D6A-4221-AB67-25E4DE633D02}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andres Calderon:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-This cell used to contain data that was deleted. This was a common source of errors when using get_data()</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="161">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -511,12 +348,6 @@
     <t>Production Pads to Treatment Facilities Trucking Arcs [-]</t>
   </si>
   <si>
-    <t>PROPRIETARY DATA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     </t>
-  </si>
-  <si>
     <t xml:space="preserve">    </t>
   </si>
   <si>
@@ -722,6 +553,12 @@
   </si>
   <si>
     <t>Elevation of a network node (including all sites)</t>
+  </si>
+  <si>
+    <t>B01</t>
+  </si>
+  <si>
+    <t>B02</t>
   </si>
 </sst>
 </file>
@@ -731,7 +568,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -798,19 +635,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -818,7 +642,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -834,12 +658,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1279,7 +1097,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1360,7 +1178,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1379,54 +1196,54 @@
     <xf numFmtId="43" fontId="3" fillId="3" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="3" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1438,6 +1255,7 @@
     <xf numFmtId="43" fontId="1" fillId="3" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1814,17 +1632,17 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.28515625" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" customWidth="1"/>
+    <col min="10" max="10" width="4.44140625" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="14"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -1836,7 +1654,7 @@
       <c r="J2" s="15"/>
       <c r="K2" s="16"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="17"/>
       <c r="C3" s="18" t="s">
         <v>10</v>
@@ -1850,7 +1668,7 @@
       <c r="J3" s="19"/>
       <c r="K3" s="20"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="17"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
@@ -1862,7 +1680,7 @@
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="17"/>
       <c r="C5" s="19" t="s">
         <v>16</v>
@@ -1876,7 +1694,7 @@
       <c r="J5" s="19"/>
       <c r="K5" s="20"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="17"/>
       <c r="C6" s="19" t="s">
         <v>14</v>
@@ -1890,7 +1708,7 @@
       <c r="J6" s="19"/>
       <c r="K6" s="20"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="17"/>
       <c r="C7" s="19" t="s">
         <v>11</v>
@@ -1904,7 +1722,7 @@
       <c r="J7" s="19"/>
       <c r="K7" s="20"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="17"/>
       <c r="C8" s="19" t="s">
         <v>12</v>
@@ -1918,7 +1736,7 @@
       <c r="J8" s="19"/>
       <c r="K8" s="20"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="17"/>
       <c r="C9" s="19" t="s">
         <v>13</v>
@@ -1932,7 +1750,7 @@
       <c r="J9" s="19"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="17"/>
       <c r="C10" s="19" t="s">
         <v>52</v>
@@ -1946,7 +1764,7 @@
       <c r="J10" s="19"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="17"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -1958,7 +1776,7 @@
       <c r="J11" s="19"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="17"/>
       <c r="C12" s="19" t="s">
         <v>17</v>
@@ -1972,7 +1790,7 @@
       <c r="J12" s="19"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="17"/>
       <c r="C13" s="19" t="s">
         <v>15</v>
@@ -1986,7 +1804,7 @@
       <c r="J13" s="19"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="17"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -1998,7 +1816,7 @@
       <c r="J14" s="19"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="17"/>
       <c r="C15" s="19" t="s">
         <v>18</v>
@@ -2012,7 +1830,7 @@
       <c r="J15" s="19"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="17"/>
       <c r="C16" s="19" t="s">
         <v>19</v>
@@ -2026,7 +1844,7 @@
       <c r="J16" s="19"/>
       <c r="K16" s="20"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B17" s="17"/>
       <c r="C17" s="19" t="s">
         <v>20</v>
@@ -2040,7 +1858,7 @@
       <c r="J17" s="19"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B18" s="17"/>
       <c r="C18" s="19" t="s">
         <v>21</v>
@@ -2054,7 +1872,7 @@
       <c r="J18" s="19"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B19" s="17"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -2066,7 +1884,7 @@
       <c r="J19" s="19"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B20" s="17"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
@@ -2078,7 +1896,7 @@
       <c r="J20" s="19"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B21" s="17"/>
       <c r="C21" s="21" t="s">
         <v>22</v>
@@ -2094,7 +1912,7 @@
       <c r="J21" s="19"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B22" s="17"/>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
@@ -2106,7 +1924,7 @@
       <c r="J22" s="19"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B23" s="17"/>
       <c r="C23" s="22" t="s">
         <v>24</v>
@@ -2122,7 +1940,7 @@
       <c r="J23" s="19"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B24" s="17"/>
       <c r="C24" s="22" t="s">
         <v>25</v>
@@ -2138,7 +1956,7 @@
       <c r="J24" s="19"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B25" s="17"/>
       <c r="C25" s="22" t="s">
         <v>26</v>
@@ -2154,7 +1972,7 @@
       <c r="J25" s="19"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B26" s="17"/>
       <c r="C26" s="22" t="s">
         <v>30</v>
@@ -2170,7 +1988,7 @@
       <c r="J26" s="19"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B27" s="17"/>
       <c r="C27" s="22" t="s">
         <v>32</v>
@@ -2186,7 +2004,7 @@
       <c r="J27" s="19"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B28" s="17"/>
       <c r="C28" s="22" t="s">
         <v>34</v>
@@ -2202,7 +2020,7 @@
       <c r="J28" s="19"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B29" s="17"/>
       <c r="C29" s="22" t="s">
         <v>35</v>
@@ -2218,7 +2036,7 @@
       <c r="J29" s="19"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B30" s="17"/>
       <c r="C30" s="22" t="s">
         <v>38</v>
@@ -2234,7 +2052,7 @@
       <c r="J30" s="19"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" s="17"/>
       <c r="C31" s="22" t="s">
         <v>40</v>
@@ -2253,7 +2071,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B32" s="17"/>
       <c r="C32" s="22" t="s">
         <v>43</v>
@@ -2269,7 +2087,7 @@
       <c r="J32" s="19"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" s="17"/>
       <c r="C33" s="22" t="s">
         <v>42</v>
@@ -2285,7 +2103,7 @@
       <c r="J33" s="19"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" s="17"/>
       <c r="C34" s="22" t="s">
         <v>46</v>
@@ -2301,7 +2119,7 @@
       <c r="J34" s="19"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" s="17"/>
       <c r="C35" s="22" t="s">
         <v>48</v>
@@ -2317,7 +2135,7 @@
       <c r="J35" s="19"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" s="17"/>
       <c r="C36" s="22" t="s">
         <v>49</v>
@@ -2333,7 +2151,7 @@
       <c r="J36" s="19"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="23"/>
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
@@ -2378,28 +2196,28 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.33203125" style="1"/>
+    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.33203125" style="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -2422,28 +2240,28 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.33203125" style="1"/>
+    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.33203125" style="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -2466,20 +2284,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="14.44140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>8</v>
@@ -2488,18 +2306,18 @@
       <c r="D2" s="7"/>
       <c r="E2" s="27"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="36"/>
     </row>
-    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -2513,90 +2331,61 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="39"/>
+    </row>
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B3" s="36">
         <v>1</v>
       </c>
-      <c r="E3" s="40">
-        <v>1</v>
-      </c>
-      <c r="F3" s="40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B4" s="11">
-        <v>1</v>
-      </c>
-      <c r="D4" s="40">
-        <f>1+1/2+1/3+1/4</f>
-        <v>2.083333333333333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="40">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2611,9 +2400,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -2634,9 +2423,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -2654,32 +2443,30 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="39"/>
+    </row>
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
@@ -2687,7 +2474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -2695,7 +2482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2703,7 +2490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -2711,7 +2498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -2719,10 +2506,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="39" t="s">
-        <v>90</v>
-      </c>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D9" s="39"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2732,35 +2517,35 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED7A596-FF30-4282-98C8-7AB378F1FE03}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED7A596-FF30-4282-98C8-7AB378F1FE03}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>75</v>
       </c>
@@ -2768,19 +2553,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
         <v>76</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
       </c>
-      <c r="D4" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2795,25 +2578,25 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -2838,20 +2621,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="16.88671875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>54</v>
@@ -2860,7 +2643,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
@@ -2869,7 +2652,7 @@
       </c>
       <c r="C3" s="36"/>
     </row>
-    <row r="4" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -2880,7 +2663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2889,7 +2672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -2898,7 +2681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -2920,351 +2703,351 @@
   </sheetPr>
   <dimension ref="A1:BA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="92.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="0.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="48" width="9.28515625" style="1"/>
-    <col min="49" max="49" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="16.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1"/>
+    <col min="4" max="4" width="92.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="0.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="48" width="9.33203125" style="1"/>
+    <col min="49" max="49" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:53" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="2" spans="1:53" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="D2" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="E2" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="50"/>
+    </row>
+    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="B3" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="51"/>
-    </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="D3" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="E3" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="G3" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="H3" s="56"/>
+      <c r="I3" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="F3" s="55" t="s">
+      <c r="K3" s="57" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="H4" s="56"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="57"/>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="58"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="60"/>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="H6" s="52"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="60"/>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" s="52"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="60"/>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="58"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="60"/>
+      <c r="AT8" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="AU8" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV8" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="AW8" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="AX8" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="AY8" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ8" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="BA8" s="37" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="F9" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="G9" s="59" t="s">
+        <v>155</v>
+      </c>
+      <c r="H9" s="52"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="60"/>
+      <c r="AT9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AU9" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AV9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AW9" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AX9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AY9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AZ9" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BA9" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" s="58"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="60"/>
+      <c r="AT10" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G3" s="56" t="s">
-        <v>119</v>
-      </c>
-      <c r="H3" s="57"/>
-      <c r="I3" s="56" t="s">
-        <v>120</v>
-      </c>
-      <c r="J3" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="K3" s="58" t="s">
+      <c r="AU10" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="B4" s="52" t="s">
+      <c r="AV10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AW10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AX10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AY10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AZ10" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="BA10" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="E11" s="62" t="s">
+        <v>144</v>
+      </c>
+      <c r="F11" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="G11" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="H11" s="61"/>
+      <c r="I11" s="65" t="s">
+        <v>146</v>
+      </c>
+      <c r="J11" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="K11" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="AU11" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="BA11" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
+      <c r="AU12" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="53" t="s">
-        <v>124</v>
-      </c>
-      <c r="E4" s="54" t="s">
-        <v>125</v>
-      </c>
-      <c r="F4" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="G4" s="56" t="s">
-        <v>126</v>
-      </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="58"/>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="B5" s="52" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="53" t="s">
-        <v>129</v>
-      </c>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="61"/>
-    </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="53" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="54" t="s">
-        <v>131</v>
-      </c>
-      <c r="F6" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="G6" s="56" t="s">
-        <v>133</v>
-      </c>
-      <c r="H6" s="53"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="61"/>
-    </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="D7" s="53" t="s">
-        <v>136</v>
-      </c>
-      <c r="E7" s="54" t="s">
-        <v>137</v>
-      </c>
-      <c r="F7" s="55" t="s">
-        <v>118</v>
-      </c>
-      <c r="G7" s="56" t="s">
-        <v>138</v>
-      </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="61"/>
-    </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="B8" s="52" t="s">
-        <v>140</v>
-      </c>
-      <c r="D8" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="61"/>
-      <c r="AT8" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="AU8" s="37" t="s">
-        <v>122</v>
-      </c>
-      <c r="AV8" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="AW8" s="37" t="s">
-        <v>130</v>
-      </c>
-      <c r="AX8" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="AY8" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="AZ8" s="37" t="s">
-        <v>154</v>
-      </c>
-      <c r="BA8" s="37" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="B9" s="52" t="s">
-        <v>155</v>
-      </c>
-      <c r="D9" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="E9" s="59" t="s">
-        <v>155</v>
-      </c>
-      <c r="F9" s="60" t="s">
-        <v>118</v>
-      </c>
-      <c r="G9" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="H9" s="53"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="61"/>
-      <c r="AT9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AU9" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AV9" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AW9" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="AX9" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="AY9" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="AZ9" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="BA9" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="B10" s="52" t="s">
-        <v>150</v>
-      </c>
-      <c r="D10" s="53" t="s">
-        <v>160</v>
-      </c>
-      <c r="E10" s="59"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="61"/>
-      <c r="AT10" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="AV10" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AW10" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="AX10" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AY10" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AZ10" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="BA10" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="B11" s="43" t="s">
-        <v>140</v>
-      </c>
-      <c r="D11" s="62" t="s">
-        <v>145</v>
-      </c>
-      <c r="E11" s="63" t="s">
+      <c r="BA12" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="F11" s="64" t="s">
-        <v>118</v>
-      </c>
-      <c r="G11" s="65" t="s">
-        <v>147</v>
-      </c>
-      <c r="H11" s="62"/>
-      <c r="I11" s="66" t="s">
-        <v>148</v>
-      </c>
-      <c r="J11" s="64" t="s">
-        <v>118</v>
-      </c>
-      <c r="K11" s="65" t="s">
-        <v>149</v>
-      </c>
-      <c r="AU11" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="BA11" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="AU12" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="BA12" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3310,25 +3093,25 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -3347,26 +3130,26 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>61</v>
@@ -3410,8 +3193,14 @@
       <c r="O2" s="27" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
@@ -3433,8 +3222,10 @@
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
       <c r="O3" s="36"/>
-    </row>
-    <row r="4" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P3" s="9"/>
+      <c r="Q3" s="36"/>
+    </row>
+    <row r="4" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -3458,8 +3249,10 @@
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
       <c r="O4" s="36"/>
-    </row>
-    <row r="5" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="9"/>
+      <c r="Q4" s="36"/>
+    </row>
+    <row r="5" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -3485,8 +3278,10 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
       <c r="O5" s="36"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="9"/>
+      <c r="Q5" s="36"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -3510,8 +3305,10 @@
       </c>
       <c r="N6" s="9"/>
       <c r="O6" s="36"/>
-    </row>
-    <row r="7" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P6" s="9"/>
+      <c r="Q6" s="36"/>
+    </row>
+    <row r="7" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -3531,6 +3328,33 @@
         <v>1</v>
       </c>
       <c r="O7" s="11">
+        <v>1</v>
+      </c>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="11">
         <v>1</v>
       </c>
     </row>
@@ -3552,23 +3376,23 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="9.28515625" style="1"/>
+    <col min="1" max="7" width="9.33203125" style="1"/>
     <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.28515625" style="1"/>
+    <col min="9" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B$9, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>#N/A</v>
+    <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B11, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
+        <v>Table of Completions Water Demand for Completions Sites over days [bbl/day]</v>
       </c>
       <c r="H1" s="39"/>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
@@ -3586,7 +3410,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -3606,7 +3430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F8" s="12"/>
     </row>
   </sheetData>
@@ -3624,29 +3448,29 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" style="8" customWidth="1"/>
     <col min="2" max="2" width="23" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.28515625" style="1"/>
+    <col min="3" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="str">
         <f>_xlfn.CONCAT( "Table of Production Rate Forecasts by Tanks and Pads"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Production Rate Forecasts by Tanks and Pads [bbl/day]</v>
       </c>
       <c r="B1" s="39"/>
     </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>93</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>95</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>56</v>
@@ -3664,7 +3488,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
@@ -3687,7 +3511,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
@@ -3710,7 +3534,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>4</v>
       </c>
@@ -3733,7 +3557,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>4</v>
       </c>
@@ -3756,7 +3580,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>4</v>
       </c>
@@ -3779,7 +3603,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
@@ -3802,7 +3626,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>5</v>
       </c>
@@ -3825,7 +3649,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>5</v>
       </c>
@@ -3848,7 +3672,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>5</v>
       </c>
@@ -3871,7 +3695,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>6</v>
       </c>
@@ -3894,7 +3718,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>6</v>
       </c>
@@ -3917,7 +3741,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
         <v>6</v>
       </c>
@@ -3940,7 +3764,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
         <v>7</v>
       </c>
@@ -3963,7 +3787,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
@@ -3986,7 +3810,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G21" s="12"/>
     </row>
   </sheetData>
@@ -4006,21 +3830,21 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="8" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="17.109375" style="8" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="str">
         <f>_xlfn.CONCAT( "Table of Production Rate Forecasts by Pads"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Production Rate Forecasts by Pads [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
@@ -4038,7 +3862,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
@@ -4058,7 +3882,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -4078,7 +3902,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -4098,7 +3922,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -4118,7 +3942,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -4138,7 +3962,7 @@
         <v>1766</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F12" s="12"/>
     </row>
   </sheetData>
@@ -4148,6 +3972,109 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1F3225-05BE-4B0D-AE83-9F04DDDFE920}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="8" width="9.33203125" style="1"/>
+    <col min="9" max="9" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.33203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B11, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
+        <v>Table of Completions Water Demand for Completions Sites over days [bbl/day]</v>
+      </c>
+      <c r="I1" s="39"/>
+    </row>
+    <row r="2" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="69" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="10">
+        <v>250</v>
+      </c>
+      <c r="D3" s="10">
+        <v>250</v>
+      </c>
+      <c r="E3" s="10">
+        <v>250</v>
+      </c>
+      <c r="F3" s="10">
+        <v>250</v>
+      </c>
+      <c r="G3" s="10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="69" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="10">
+        <v>250</v>
+      </c>
+      <c r="D4" s="10">
+        <v>250</v>
+      </c>
+      <c r="E4" s="10">
+        <v>250</v>
+      </c>
+      <c r="F4" s="10">
+        <v>250</v>
+      </c>
+      <c r="G4" s="10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G8" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16A47F7-A2FF-4DEE-B278-2DA8AB93D602}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -4158,21 +4085,21 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="8"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="9.33203125" style="8"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="str">
         <f>_xlfn.CONCAT( "Table of Flowback Rate Forecasts by Pads"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Flowback Rate Forecasts by Pads [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
@@ -4190,7 +4117,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4210,7 +4137,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F8" s="12"/>
     </row>
   </sheetData>
@@ -4219,7 +4146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4228,12 +4155,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Initial Disposal Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Initial Disposal Capacity [bbl/day]</v>
@@ -4241,16 +4168,16 @@
       <c r="B1" s="39"/>
       <c r="D1" s="39"/>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D2" s="39"/>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>54</v>
       </c>
@@ -4258,7 +4185,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
         <v>55</v>
       </c>
@@ -4267,7 +4194,7 @@
       </c>
       <c r="D4" s="39"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="39"/>
       <c r="B6" s="39"/>
       <c r="D6" s="39"/>
@@ -4278,7 +4205,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59865970-D83F-46CB-8781-62CE35DBF4B5}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4287,9 +4214,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Table of Reuse Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Reuse Capacity [bbl/day]</v>
@@ -4300,7 +4227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4309,21 +4236,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Availability"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Freshwater Sourcing Availability [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>56</v>
@@ -4341,7 +4268,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>75</v>
       </c>
@@ -4361,7 +4288,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
         <v>76</v>
       </c>
@@ -4381,75 +4308,8 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F9" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA48CF8D-5373-4539-A55F-3258FEB20DFB}">
-  <sheetPr>
-    <tabColor rgb="FFD9C6FE"/>
-  </sheetPr>
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.140625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Completions Pad Storage Capacity [bbl]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="42">
-        <v>10000</v>
-      </c>
-      <c r="C3" s="42">
-        <v>10000</v>
-      </c>
-      <c r="D3" s="42">
-        <v>10000</v>
-      </c>
-      <c r="E3" s="42">
-        <v>10000</v>
-      </c>
-      <c r="F3" s="43">
-        <v>10000</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4468,39 +4328,39 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="9.28515625" style="1"/>
-    <col min="10" max="10" width="11.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="4.5703125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="9" width="9.33203125" style="1"/>
+    <col min="10" max="10" width="11.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5546875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="39"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="39"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -4508,12 +4368,12 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="39"/>
       <c r="C10" s="39"/>
     </row>
@@ -4525,6 +4385,73 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA48CF8D-5373-4539-A55F-3258FEB20DFB}">
+  <sheetPr>
+    <tabColor rgb="FFD9C6FE"/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Completions Pad Storage Capacity [bbl]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="41">
+        <v>10000</v>
+      </c>
+      <c r="C3" s="41">
+        <v>10000</v>
+      </c>
+      <c r="D3" s="41">
+        <v>10000</v>
+      </c>
+      <c r="E3" s="41">
+        <v>10000</v>
+      </c>
+      <c r="F3" s="42">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4533,27 +4460,27 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Pad Offloading Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Pad Offloading Capacity [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4567,7 +4494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EB27A2-91E8-4B14-8B2B-D8903B8CA8E8}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4576,9 +4503,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Production Tank Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Production Tank Capacity [bbl]</v>
@@ -4589,7 +4516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4600,26 +4527,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Disposal Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Disposal Operational Cost [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>54</v>
       </c>
@@ -4627,7 +4554,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
         <v>55</v>
       </c>
@@ -4641,7 +4568,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74013BD9-1426-4BFB-8D02-5A2A33597048}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4652,13 +4579,13 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4669,27 +4596,27 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="17.88671875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Reuse Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Reuse Operational Cost [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4703,7 +4630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FF3D68-9420-4DF5-8A14-DD803657C7A5}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4714,26 +4641,26 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Piping Operational Costs [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Piping Operational Costs [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>75</v>
       </c>
@@ -4741,7 +4668,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
         <v>76</v>
       </c>
@@ -4755,7 +4682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4766,27 +4693,27 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="17.5546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Freshwater Sourcing Cost [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>75</v>
       </c>
@@ -4794,7 +4721,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
         <v>76</v>
       </c>
@@ -4808,7 +4735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2915391D-1D4E-446C-B6C1-F25D75A5D98F}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4819,23 +4746,23 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.28515625" style="1"/>
+    <col min="2" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity over Time [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Completions Pad Storage Capacity over Time [bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="40" t="s">
         <v>56</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -4851,23 +4778,23 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="42">
+      <c r="B3" s="41">
         <v>250</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="41">
         <v>250</v>
       </c>
-      <c r="D3" s="42">
+      <c r="D3" s="41">
         <v>250</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="41">
         <v>250</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="42">
         <v>250</v>
       </c>
     </row>
@@ -4877,7 +4804,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4888,26 +4815,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Trucking Hourly Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", "hour","]")</f>
         <v>Table of Trucking Hourly Cost [USD/hour]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>8</v>
       </c>
@@ -4915,7 +4842,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>75</v>
       </c>
@@ -4923,7 +4850,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>76</v>
       </c>
@@ -4931,7 +4858,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>3</v>
       </c>
@@ -4939,7 +4866,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>4</v>
       </c>
@@ -4947,7 +4874,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
@@ -4955,7 +4882,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>6</v>
       </c>
@@ -4963,235 +4890,13 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="33" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11">
         <v>92</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:I17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="6" width="9.28515625" style="1"/>
-    <col min="7" max="8" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.28515625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9">
-        <v>1</v>
-      </c>
-      <c r="H3" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="I3" s="36"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="H4" s="9">
-        <v>1</v>
-      </c>
-      <c r="I4" s="36">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9">
-        <v>2</v>
-      </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="36">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="36">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9">
-        <v>3</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9">
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="H8" s="9">
-        <v>2</v>
-      </c>
-      <c r="I8" s="36"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9">
-        <v>2</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="36"/>
-    </row>
-    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="36"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="36"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="11"/>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5204,46 +4909,46 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.28515625" style="1"/>
-    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.28515625" style="1"/>
-    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="2" width="9.33203125" style="1"/>
+    <col min="3" max="3" width="3.5546875" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.33203125" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5546875" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D4" s="12"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>64</v>
       </c>
@@ -5251,54 +4956,64 @@
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -5309,6 +5024,228 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2" max="6" width="9.33203125" style="1"/>
+    <col min="7" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.33203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="I3" s="36"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="H4" s="9">
+        <v>1</v>
+      </c>
+      <c r="I4" s="36">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9">
+        <v>2</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="36">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9">
+        <v>3</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="H8" s="9">
+        <v>2</v>
+      </c>
+      <c r="I8" s="36"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9">
+        <v>2</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="36"/>
+    </row>
+    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="36"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="36"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G17" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4E39D9-E2B5-4E92-A460-6BB588CED0C5}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -5319,35 +5256,35 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
@@ -5359,7 +5296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3E2031-E70C-46E6-B55F-07206AFEE600}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -5370,71 +5307,71 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Table of Water Quality of Produced Water and Flowback Water [",VLOOKUP("concentration", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Water Quality of Produced Water and Flowback Water [mg/liter]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="67">
+      <c r="B3" s="66">
         <v>142277</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="68">
+      <c r="B4" s="67">
         <v>140998</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="68">
+      <c r="B5" s="67">
         <v>172490.2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="68">
+      <c r="B6" s="67">
         <v>257547</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="68">
+      <c r="B7" s="67">
         <v>241833.8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="69">
+      <c r="B8" s="68">
         <v>188503.7</v>
       </c>
     </row>
@@ -5444,7 +5381,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465369F7-E9A8-4A2B-BBBA-6F1C07C7C51F}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -5455,29 +5392,29 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Table of Initial Water Quality at Storage [",VLOOKUP("concentration", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Initial Water Quality at Storage [mg/liter]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="44" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="45"/>
-      <c r="B3" s="46"/>
+      <c r="B2" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="44"/>
+      <c r="B3" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5496,30 +5433,30 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.33203125" style="1"/>
+    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.33203125" style="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
@@ -5542,28 +5479,28 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="4.42578125" style="1" customWidth="1"/>
-    <col min="5" max="14" width="9.28515625" style="1"/>
-    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.5703125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="3" width="9.33203125" style="1"/>
+    <col min="4" max="4" width="4.44140625" style="1" customWidth="1"/>
+    <col min="5" max="14" width="9.33203125" style="1"/>
+    <col min="15" max="15" width="12.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.5546875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>55</v>
       </c>
@@ -5586,30 +5523,30 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.33203125" style="1"/>
+    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.33203125" style="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>76</v>
       </c>
@@ -5635,28 +5572,28 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.33203125" style="1"/>
+    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.33203125" style="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -5679,32 +5616,32 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="9.28515625" style="1"/>
-    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.33203125" style="1"/>
+    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.28515625" style="1"/>
-    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.28515625" style="1"/>
+    <col min="6" max="13" width="9.33203125" style="1"/>
+    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>

</xml_diff>

<commit_message>
Implement freshwater quality for operational model
</commit_message>
<xml_diff>
--- a/pareto/case_studies/operational_generic_case_study.xlsx
+++ b/pareto/case_studies/operational_generic_case_study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E48321-923B-48F5-8BE6-3E12B24E4753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3917B8-5013-4662-83BA-991624C5E1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="770" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="770" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -20,42 +20,44 @@
     <sheet name="CompletionsPads" sheetId="3" r:id="rId5"/>
     <sheet name="SWDSites" sheetId="4" r:id="rId6"/>
     <sheet name="FreshwaterSources" sheetId="35" r:id="rId7"/>
-    <sheet name="StorageSites" sheetId="36" r:id="rId8"/>
-    <sheet name="TreatmentSites" sheetId="37" r:id="rId9"/>
-    <sheet name="ReuseOptions" sheetId="38" r:id="rId10"/>
-    <sheet name="NetworkNodes" sheetId="39" r:id="rId11"/>
-    <sheet name="RCA" sheetId="67" r:id="rId12"/>
-    <sheet name="FCA" sheetId="41" r:id="rId13"/>
-    <sheet name="PRT" sheetId="59" r:id="rId14"/>
-    <sheet name="CRT" sheetId="60" r:id="rId15"/>
-    <sheet name="PCT" sheetId="42" r:id="rId16"/>
-    <sheet name="FCT" sheetId="53" r:id="rId17"/>
-    <sheet name="CCT" sheetId="57" r:id="rId18"/>
-    <sheet name="PKT" sheetId="43" r:id="rId19"/>
-    <sheet name="CKT" sheetId="44" r:id="rId20"/>
-    <sheet name="PAL" sheetId="45" r:id="rId21"/>
-    <sheet name="CompletionsDemand" sheetId="8" r:id="rId22"/>
-    <sheet name="ProductionRates" sheetId="40" r:id="rId23"/>
-    <sheet name="PadRates" sheetId="56" r:id="rId24"/>
-    <sheet name="TankFlowbackRates" sheetId="74" r:id="rId25"/>
-    <sheet name="FlowbackRates" sheetId="58" r:id="rId26"/>
-    <sheet name="DisposalCapacity" sheetId="46" r:id="rId27"/>
-    <sheet name="TreatmentCapacity" sheetId="62" r:id="rId28"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId29"/>
-    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId30"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId31"/>
-    <sheet name="ProductionTankCapacity" sheetId="61" r:id="rId32"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId33"/>
-    <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId34"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId35"/>
-    <sheet name="PipelineOperationalCost" sheetId="54" r:id="rId36"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId37"/>
-    <sheet name="PadStorageCost" sheetId="70" r:id="rId38"/>
-    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId39"/>
-    <sheet name="TruckingTime" sheetId="7" r:id="rId40"/>
-    <sheet name="TreatmentEfficiency" sheetId="69" r:id="rId41"/>
-    <sheet name="PadWaterQuality" sheetId="71" r:id="rId42"/>
-    <sheet name="StorageInitialWaterQuality" sheetId="72" r:id="rId43"/>
+    <sheet name="WaterQualityComponents" sheetId="75" r:id="rId8"/>
+    <sheet name="StorageSites" sheetId="36" r:id="rId9"/>
+    <sheet name="TreatmentSites" sheetId="37" r:id="rId10"/>
+    <sheet name="ReuseOptions" sheetId="38" r:id="rId11"/>
+    <sheet name="NetworkNodes" sheetId="39" r:id="rId12"/>
+    <sheet name="RCA" sheetId="67" r:id="rId13"/>
+    <sheet name="FCA" sheetId="41" r:id="rId14"/>
+    <sheet name="PRT" sheetId="59" r:id="rId15"/>
+    <sheet name="CRT" sheetId="60" r:id="rId16"/>
+    <sheet name="PCT" sheetId="42" r:id="rId17"/>
+    <sheet name="FCT" sheetId="53" r:id="rId18"/>
+    <sheet name="CCT" sheetId="57" r:id="rId19"/>
+    <sheet name="PKT" sheetId="43" r:id="rId20"/>
+    <sheet name="CKT" sheetId="44" r:id="rId21"/>
+    <sheet name="PAL" sheetId="45" r:id="rId22"/>
+    <sheet name="CompletionsDemand" sheetId="8" r:id="rId23"/>
+    <sheet name="ProductionRates" sheetId="40" r:id="rId24"/>
+    <sheet name="PadRates" sheetId="56" r:id="rId25"/>
+    <sheet name="TankFlowbackRates" sheetId="74" r:id="rId26"/>
+    <sheet name="FlowbackRates" sheetId="58" r:id="rId27"/>
+    <sheet name="DisposalCapacity" sheetId="46" r:id="rId28"/>
+    <sheet name="TreatmentCapacity" sheetId="62" r:id="rId29"/>
+    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId30"/>
+    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId31"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId32"/>
+    <sheet name="ProductionTankCapacity" sheetId="61" r:id="rId33"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId34"/>
+    <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId35"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId36"/>
+    <sheet name="PipelineOperationalCost" sheetId="54" r:id="rId37"/>
+    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId38"/>
+    <sheet name="PadStorageCost" sheetId="70" r:id="rId39"/>
+    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId40"/>
+    <sheet name="TruckingTime" sheetId="7" r:id="rId41"/>
+    <sheet name="TreatmentEfficiency" sheetId="69" r:id="rId42"/>
+    <sheet name="FreshwaterQuality" sheetId="76" r:id="rId43"/>
+    <sheet name="PadWaterQuality" sheetId="71" r:id="rId44"/>
+    <sheet name="StorageInitialWaterQuality" sheetId="72" r:id="rId45"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -76,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="162">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -559,6 +561,9 @@
   </si>
   <si>
     <t>B02</t>
+  </si>
+  <si>
+    <t>List of all Water Quality Components [-]</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1104,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1256,6 +1261,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1634,15 +1645,15 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.33203125" customWidth="1"/>
-    <col min="10" max="10" width="4.44140625" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="14"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -1654,7 +1665,7 @@
       <c r="J2" s="15"/>
       <c r="K2" s="16"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="17"/>
       <c r="C3" s="18" t="s">
         <v>10</v>
@@ -1668,7 +1679,7 @@
       <c r="J3" s="19"/>
       <c r="K3" s="20"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="17"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
@@ -1680,7 +1691,7 @@
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
       <c r="C5" s="19" t="s">
         <v>16</v>
@@ -1694,7 +1705,7 @@
       <c r="J5" s="19"/>
       <c r="K5" s="20"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="17"/>
       <c r="C6" s="19" t="s">
         <v>14</v>
@@ -1708,7 +1719,7 @@
       <c r="J6" s="19"/>
       <c r="K6" s="20"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="17"/>
       <c r="C7" s="19" t="s">
         <v>11</v>
@@ -1722,7 +1733,7 @@
       <c r="J7" s="19"/>
       <c r="K7" s="20"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="17"/>
       <c r="C8" s="19" t="s">
         <v>12</v>
@@ -1736,7 +1747,7 @@
       <c r="J8" s="19"/>
       <c r="K8" s="20"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="17"/>
       <c r="C9" s="19" t="s">
         <v>13</v>
@@ -1750,7 +1761,7 @@
       <c r="J9" s="19"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
       <c r="C10" s="19" t="s">
         <v>52</v>
@@ -1764,7 +1775,7 @@
       <c r="J10" s="19"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="17"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -1776,7 +1787,7 @@
       <c r="J11" s="19"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="17"/>
       <c r="C12" s="19" t="s">
         <v>17</v>
@@ -1790,7 +1801,7 @@
       <c r="J12" s="19"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="17"/>
       <c r="C13" s="19" t="s">
         <v>15</v>
@@ -1804,7 +1815,7 @@
       <c r="J13" s="19"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="17"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -1816,7 +1827,7 @@
       <c r="J14" s="19"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="17"/>
       <c r="C15" s="19" t="s">
         <v>18</v>
@@ -1830,7 +1841,7 @@
       <c r="J15" s="19"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="17"/>
       <c r="C16" s="19" t="s">
         <v>19</v>
@@ -1844,7 +1855,7 @@
       <c r="J16" s="19"/>
       <c r="K16" s="20"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="17"/>
       <c r="C17" s="19" t="s">
         <v>20</v>
@@ -1858,7 +1869,7 @@
       <c r="J17" s="19"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="17"/>
       <c r="C18" s="19" t="s">
         <v>21</v>
@@ -1872,7 +1883,7 @@
       <c r="J18" s="19"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="17"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -1884,7 +1895,7 @@
       <c r="J19" s="19"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="17"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
@@ -1896,7 +1907,7 @@
       <c r="J20" s="19"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="17"/>
       <c r="C21" s="21" t="s">
         <v>22</v>
@@ -1912,7 +1923,7 @@
       <c r="J21" s="19"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="17"/>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
@@ -1924,7 +1935,7 @@
       <c r="J22" s="19"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="17"/>
       <c r="C23" s="22" t="s">
         <v>24</v>
@@ -1940,7 +1951,7 @@
       <c r="J23" s="19"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="17"/>
       <c r="C24" s="22" t="s">
         <v>25</v>
@@ -1956,7 +1967,7 @@
       <c r="J24" s="19"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="17"/>
       <c r="C25" s="22" t="s">
         <v>26</v>
@@ -1972,7 +1983,7 @@
       <c r="J25" s="19"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="17"/>
       <c r="C26" s="22" t="s">
         <v>30</v>
@@ -1988,7 +1999,7 @@
       <c r="J26" s="19"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="17"/>
       <c r="C27" s="22" t="s">
         <v>32</v>
@@ -2004,7 +2015,7 @@
       <c r="J27" s="19"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="17"/>
       <c r="C28" s="22" t="s">
         <v>34</v>
@@ -2020,7 +2031,7 @@
       <c r="J28" s="19"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="17"/>
       <c r="C29" s="22" t="s">
         <v>35</v>
@@ -2036,7 +2047,7 @@
       <c r="J29" s="19"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="17"/>
       <c r="C30" s="22" t="s">
         <v>38</v>
@@ -2052,7 +2063,7 @@
       <c r="J30" s="19"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="17"/>
       <c r="C31" s="22" t="s">
         <v>40</v>
@@ -2071,7 +2082,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="17"/>
       <c r="C32" s="22" t="s">
         <v>43</v>
@@ -2087,7 +2098,7 @@
       <c r="J32" s="19"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="17"/>
       <c r="C33" s="22" t="s">
         <v>42</v>
@@ -2103,7 +2114,7 @@
       <c r="J33" s="19"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="17"/>
       <c r="C34" s="22" t="s">
         <v>46</v>
@@ -2119,7 +2130,7 @@
       <c r="J34" s="19"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="17"/>
       <c r="C35" s="22" t="s">
         <v>48</v>
@@ -2135,7 +2146,7 @@
       <c r="J35" s="19"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="17"/>
       <c r="C36" s="22" t="s">
         <v>49</v>
@@ -2151,7 +2162,7 @@
       <c r="J36" s="19"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="23"/>
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
@@ -2186,6 +2197,54 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF69D0FC-C70F-430B-9882-945A087A2D92}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:P3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A85E027-57F4-45A3-888B-4C0E11BBDC89}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2196,28 +2255,28 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.33203125" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.33203125" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -2229,7 +2288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F8A809-1347-42CB-A460-105FB2B000F6}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2240,28 +2299,28 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.33203125" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.33203125" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -2273,7 +2332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19482E4D-5604-4B83-9F7A-0225AC5DE7E0}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2284,18 +2343,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>101</v>
       </c>
@@ -2306,7 +2365,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="27"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>102</v>
       </c>
@@ -2315,7 +2374,7 @@
       <c r="D3" s="9"/>
       <c r="E3" s="36"/>
     </row>
-    <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>103</v>
       </c>
@@ -2330,7 +2389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2341,19 +2400,19 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B1" s="39"/>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>96</v>
       </c>
@@ -2364,7 +2423,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>75</v>
       </c>
@@ -2375,7 +2434,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>76</v>
       </c>
@@ -2389,7 +2448,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC3797B-8D14-4FB6-B72A-3C0C4341EC79}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2400,9 +2459,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -2412,7 +2471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F1A6821-D55E-4269-AC7B-EA9C0F0EC2AD}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2423,9 +2482,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -2435,7 +2494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6ED8ED-0A77-4974-A7C2-D2B875DA1401}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2446,19 +2505,19 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E1" s="39"/>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>91</v>
       </c>
@@ -2466,7 +2525,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
@@ -2474,7 +2533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -2482,7 +2541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2490,7 +2549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -2498,7 +2557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -2506,7 +2565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" s="39"/>
     </row>
   </sheetData>
@@ -2516,7 +2575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED7A596-FF30-4282-98C8-7AB378F1FE03}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2527,17 +2586,17 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>96</v>
       </c>
@@ -2545,7 +2604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>75</v>
       </c>
@@ -2553,7 +2612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>76</v>
       </c>
@@ -2567,7 +2626,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16082D3-6CFF-4538-9513-170B327E5C50}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2578,17 +2637,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>94</v>
       </c>
@@ -2596,97 +2655,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="11">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AE275C-BC38-44C0-8EFB-EA0A3ABCF1EE}">
-  <sheetPr>
-    <tabColor theme="9" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.88671875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="36"/>
-    </row>
-    <row r="4" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2707,34 +2680,34 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="92.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="0.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="48" width="9.33203125" style="1"/>
-    <col min="49" max="49" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="92.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="0.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="48" width="9.28515625" style="1"/>
+    <col min="49" max="49" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:53" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>109</v>
       </c>
@@ -2754,7 +2727,7 @@
       <c r="J2" s="48"/>
       <c r="K2" s="50"/>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>113</v>
       </c>
@@ -2784,7 +2757,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>120</v>
       </c>
@@ -2808,7 +2781,7 @@
       <c r="J4" s="55"/>
       <c r="K4" s="57"/>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>125</v>
       </c>
@@ -2826,7 +2799,7 @@
       <c r="J5" s="59"/>
       <c r="K5" s="60"/>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>128</v>
       </c>
@@ -2850,7 +2823,7 @@
       <c r="J6" s="59"/>
       <c r="K6" s="60"/>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>132</v>
       </c>
@@ -2874,7 +2847,7 @@
       <c r="J7" s="59"/>
       <c r="K7" s="60"/>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>137</v>
       </c>
@@ -2916,7 +2889,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>152</v>
       </c>
@@ -2964,7 +2937,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>157</v>
       </c>
@@ -3006,7 +2979,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
         <v>141</v>
       </c>
@@ -3042,7 +3015,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="AU12" s="1" t="s">
         <v>123</v>
       </c>
@@ -3083,6 +3056,92 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AE275C-BC38-44C0-8EFB-EA0A3ABCF1EE}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="36"/>
+    </row>
+    <row r="4" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="37"/>
+      <c r="C6" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90457C74-863B-4C67-B58B-571271FAEA0E}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -3093,17 +3152,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>94</v>
       </c>
@@ -3111,7 +3170,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -3125,7 +3184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABD83BE-FC18-4B07-A835-FE113535C483}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -3136,18 +3195,18 @@
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>91</v>
       </c>
@@ -3200,7 +3259,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
@@ -3225,7 +3284,7 @@
       <c r="P3" s="9"/>
       <c r="Q3" s="36"/>
     </row>
-    <row r="4" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -3252,7 +3311,7 @@
       <c r="P4" s="9"/>
       <c r="Q4" s="36"/>
     </row>
-    <row r="5" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -3281,7 +3340,7 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="36"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -3308,7 +3367,7 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="36"/>
     </row>
-    <row r="7" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -3333,7 +3392,7 @@
       <c r="P7" s="10"/>
       <c r="Q7" s="11"/>
     </row>
-    <row r="8" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
@@ -3365,7 +3424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3376,21 +3435,21 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="9.33203125" style="1"/>
+    <col min="1" max="7" width="9.28515625" style="1"/>
     <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.33203125" style="1"/>
+    <col min="9" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B11, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
         <v>Table of Completions Water Demand for Completions Sites over days [bbl/day]</v>
       </c>
       <c r="H1" s="39"/>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>94</v>
       </c>
@@ -3410,7 +3469,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -3430,7 +3489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F8" s="12"/>
     </row>
   </sheetData>
@@ -3440,7 +3499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF09514F-DAFF-4764-9C34-8E43F32C86F9}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3451,21 +3510,21 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="8" customWidth="1"/>
     <col min="2" max="2" width="23" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.33203125" style="1"/>
+    <col min="3" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="str">
         <f>_xlfn.CONCAT( "Table of Production Rate Forecasts by Tanks and Pads"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Production Rate Forecasts by Tanks and Pads [bbl/day]</v>
       </c>
       <c r="B1" s="39"/>
     </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>91</v>
       </c>
@@ -3488,7 +3547,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
@@ -3511,7 +3570,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
@@ -3534,7 +3593,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>4</v>
       </c>
@@ -3557,7 +3616,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>4</v>
       </c>
@@ -3580,7 +3639,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>4</v>
       </c>
@@ -3603,7 +3662,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
@@ -3626,7 +3685,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>5</v>
       </c>
@@ -3649,7 +3708,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>5</v>
       </c>
@@ -3672,7 +3731,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>5</v>
       </c>
@@ -3695,7 +3754,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>6</v>
       </c>
@@ -3718,7 +3777,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>6</v>
       </c>
@@ -3741,7 +3800,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>6</v>
       </c>
@@ -3764,7 +3823,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>7</v>
       </c>
@@ -3787,7 +3846,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
@@ -3810,7 +3869,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G21" s="12"/>
     </row>
   </sheetData>
@@ -3819,7 +3878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AE5548-F8CC-426B-BF72-21E59575CB18}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3830,19 +3889,19 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" style="8" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="17.140625" style="8" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="str">
         <f>_xlfn.CONCAT( "Table of Production Rate Forecasts by Pads"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Production Rate Forecasts by Pads [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>91</v>
       </c>
@@ -3862,7 +3921,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
@@ -3882,7 +3941,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -3902,7 +3961,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -3922,7 +3981,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -3942,7 +4001,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -3962,7 +4021,7 @@
         <v>1766</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F12" s="12"/>
     </row>
   </sheetData>
@@ -3971,7 +4030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1F3225-05BE-4B0D-AE83-9F04DDDFE920}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3982,21 +4041,21 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="9.33203125" style="1"/>
+    <col min="1" max="8" width="9.28515625" style="1"/>
     <col min="9" max="9" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.33203125" style="1"/>
+    <col min="10" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B11, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
         <v>Table of Completions Water Demand for Completions Sites over days [bbl/day]</v>
       </c>
       <c r="I1" s="39"/>
     </row>
-    <row r="2" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>94</v>
       </c>
@@ -4019,7 +4078,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -4042,7 +4101,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -4065,7 +4124,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G8" s="12"/>
     </row>
   </sheetData>
@@ -4074,7 +4133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16A47F7-A2FF-4DEE-B278-2DA8AB93D602}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -4085,19 +4144,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="8"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="9.28515625" style="8"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="str">
         <f>_xlfn.CONCAT( "Table of Flowback Rate Forecasts by Pads"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Flowback Rate Forecasts by Pads [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>94</v>
       </c>
@@ -4117,7 +4176,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4137,7 +4196,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F8" s="12"/>
     </row>
   </sheetData>
@@ -4146,7 +4205,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4155,12 +4214,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Initial Disposal Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Initial Disposal Capacity [bbl/day]</v>
@@ -4168,7 +4227,7 @@
       <c r="B1" s="39"/>
       <c r="D1" s="39"/>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>95</v>
       </c>
@@ -4177,7 +4236,7 @@
       </c>
       <c r="D2" s="39"/>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>54</v>
       </c>
@@ -4185,7 +4244,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>55</v>
       </c>
@@ -4194,7 +4253,7 @@
       </c>
       <c r="D4" s="39"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="39"/>
       <c r="B6" s="39"/>
       <c r="D6" s="39"/>
@@ -4205,7 +4264,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59865970-D83F-46CB-8781-62CE35DBF4B5}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4214,9 +4273,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Table of Reuse Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Reuse Capacity [bbl/day]</v>
@@ -4224,96 +4283,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
-  <sheetPr>
-    <tabColor rgb="FFD9C6FE"/>
-  </sheetPr>
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Availability"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Freshwater Sourcing Availability [bbl/day]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="9">
-        <v>30000</v>
-      </c>
-      <c r="C3" s="9">
-        <v>30000</v>
-      </c>
-      <c r="D3" s="9">
-        <v>30000</v>
-      </c>
-      <c r="E3" s="9">
-        <v>30000</v>
-      </c>
-      <c r="F3" s="36">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="10">
-        <v>20000</v>
-      </c>
-      <c r="C4" s="10">
-        <v>20000</v>
-      </c>
-      <c r="D4" s="10">
-        <v>20000</v>
-      </c>
-      <c r="E4" s="10">
-        <v>20000</v>
-      </c>
-      <c r="F4" s="11">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F9" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4328,39 +4297,39 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="9.33203125" style="1"/>
-    <col min="10" max="10" width="11.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="4.5546875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="9" width="9.28515625" style="1"/>
+    <col min="10" max="10" width="11.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="39"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="39"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -4368,12 +4337,12 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="39"/>
       <c r="C10" s="39"/>
     </row>
@@ -4385,6 +4354,96 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
+  <sheetPr>
+    <tabColor rgb="FFD9C6FE"/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Availability"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of Freshwater Sourcing Availability [bbl/day]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="9">
+        <v>30000</v>
+      </c>
+      <c r="C3" s="9">
+        <v>30000</v>
+      </c>
+      <c r="D3" s="9">
+        <v>30000</v>
+      </c>
+      <c r="E3" s="9">
+        <v>30000</v>
+      </c>
+      <c r="F3" s="36">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="10">
+        <v>20000</v>
+      </c>
+      <c r="C4" s="10">
+        <v>20000</v>
+      </c>
+      <c r="D4" s="10">
+        <v>20000</v>
+      </c>
+      <c r="E4" s="10">
+        <v>20000</v>
+      </c>
+      <c r="F4" s="11">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA48CF8D-5373-4539-A55F-3258FEB20DFB}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4393,19 +4452,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="15.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Completions Pad Storage Capacity [bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>94</v>
       </c>
@@ -4425,7 +4484,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4451,7 +4510,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4460,19 +4519,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Pad Offloading Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Pad Offloading Capacity [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>94</v>
       </c>
@@ -4480,7 +4539,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4494,7 +4553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EB27A2-91E8-4B14-8B2B-D8903B8CA8E8}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4503,9 +4562,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Production Tank Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Production Tank Capacity [bbl]</v>
@@ -4516,7 +4575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4527,18 +4586,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Disposal Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Disposal Operational Cost [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>95</v>
       </c>
@@ -4546,7 +4605,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>54</v>
       </c>
@@ -4554,7 +4613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>55</v>
       </c>
@@ -4568,7 +4627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74013BD9-1426-4BFB-8D02-5A2A33597048}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4579,13 +4638,13 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4596,19 +4655,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Reuse Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Reuse Operational Cost [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>94</v>
       </c>
@@ -4616,7 +4675,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4630,7 +4689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FF3D68-9420-4DF5-8A14-DD803657C7A5}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4641,18 +4700,18 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Piping Operational Costs [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Piping Operational Costs [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>96</v>
       </c>
@@ -4660,7 +4719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>75</v>
       </c>
@@ -4668,7 +4727,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>76</v>
       </c>
@@ -4682,7 +4741,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4693,19 +4752,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Freshwater Sourcing Cost [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>96</v>
       </c>
@@ -4713,7 +4772,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>75</v>
       </c>
@@ -4721,7 +4780,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>76</v>
       </c>
@@ -4735,7 +4794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2915391D-1D4E-446C-B6C1-F25D75A5D98F}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4746,19 +4805,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity over Time [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Completions Pad Storage Capacity over Time [bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>94</v>
       </c>
@@ -4778,7 +4837,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -4796,106 +4855,6 @@
       </c>
       <c r="F3" s="42">
         <v>250</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Trucking Hourly Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", "hour","]")</f>
-        <v>Table of Trucking Hourly Cost [USD/hour]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="36">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="36">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="36">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="36">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="36">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="36">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="36">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="11">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -4915,40 +4874,40 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.33203125" style="1"/>
-    <col min="3" max="3" width="3.5546875" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.33203125" style="1"/>
-    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5546875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="2" width="9.28515625" style="1"/>
+    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.28515625" style="1"/>
+    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>63</v>
       </c>
       <c r="D4" s="12"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>64</v>
       </c>
@@ -4956,62 +4915,62 @@
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>160</v>
       </c>
@@ -5024,6 +4983,106 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Trucking Hourly Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", "hour","]")</f>
+        <v>Table of Trucking Hourly Cost [USD/hour]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="36">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="36">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="36">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="36">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="36">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="36">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="36">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -5034,20 +5093,20 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2" max="6" width="9.33203125" style="1"/>
-    <col min="7" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2" max="6" width="9.28515625" style="1"/>
+    <col min="7" max="8" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>99</v>
       </c>
@@ -5076,7 +5135,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -5093,7 +5152,7 @@
       </c>
       <c r="I3" s="36"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -5112,7 +5171,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -5129,7 +5188,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -5146,7 +5205,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -5163,7 +5222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -5180,7 +5239,7 @@
       </c>
       <c r="I8" s="36"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>75</v>
       </c>
@@ -5195,7 +5254,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="36"/>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>76</v>
       </c>
@@ -5210,7 +5269,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="36"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
@@ -5223,7 +5282,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="36"/>
     </row>
-    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>55</v>
       </c>
@@ -5236,7 +5295,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="11"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" s="13"/>
     </row>
   </sheetData>
@@ -5245,7 +5304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4E39D9-E2B5-4E92-A460-6BB588CED0C5}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -5256,17 +5315,17 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>101</v>
       </c>
@@ -5274,7 +5333,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>102</v>
       </c>
@@ -5282,7 +5341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>103</v>
       </c>
@@ -5296,7 +5355,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE408470-1FBA-45E4-B7D1-937724BB7595}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Water Quality of Freshwater Sources [",VLOOKUP("concentration", Units!$A$2:$B$11, 2, FALSE),"]")</f>
+        <v>Table of Water Quality of Freshwater Sources [mg/liter]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="71">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3E2031-E70C-46E6-B55F-07206AFEE600}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -5307,19 +5418,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Table of Water Quality of Produced Water and Flowback Water [",VLOOKUP("concentration", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Water Quality of Produced Water and Flowback Water [mg/liter]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>106</v>
       </c>
@@ -5327,7 +5438,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
@@ -5335,7 +5446,7 @@
         <v>142277</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -5343,7 +5454,7 @@
         <v>140998</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -5351,7 +5462,7 @@
         <v>172490.2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -5359,7 +5470,7 @@
         <v>257547</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>7</v>
       </c>
@@ -5367,7 +5478,7 @@
         <v>241833.8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
@@ -5381,7 +5492,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465369F7-E9A8-4A2B-BBBA-6F1C07C7C51F}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -5392,19 +5503,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Table of Initial Water Quality at Storage [",VLOOKUP("concentration", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Initial Water Quality at Storage [mg/liter]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>107</v>
       </c>
@@ -5412,7 +5523,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="44"/>
       <c r="B3" s="45"/>
     </row>
@@ -5433,30 +5544,30 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.33203125" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.33203125" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
@@ -5479,28 +5590,28 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="4.44140625" style="1" customWidth="1"/>
-    <col min="5" max="14" width="9.33203125" style="1"/>
-    <col min="15" max="15" width="12.109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.5546875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5" max="14" width="9.28515625" style="1"/>
+    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.5703125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>55</v>
       </c>
@@ -5520,33 +5631,33 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.33203125" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.33203125" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>76</v>
       </c>
@@ -5562,6 +5673,37 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B022271-250D-45AC-910B-001BCA072919}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0D7E5C-CD82-4DB8-A226-3E1C788BA0DC}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -5572,77 +5714,29 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.33203125" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.33203125" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF69D0FC-C70F-430B-9882-945A087A2D92}">
-  <sheetPr>
-    <tabColor theme="9" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:P3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.33203125" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.33203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>

</xml_diff>

<commit_message>
Change all references to fresh water to external water
</commit_message>
<xml_diff>
--- a/pareto/case_studies/operational_generic_case_study.xlsx
+++ b/pareto/case_studies/operational_generic_case_study.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3917B8-5013-4662-83BA-991624C5E1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CE4AC1-C8F3-4047-87A2-883EE564938B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="770" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="ProductionTanks" sheetId="34" r:id="rId4"/>
     <sheet name="CompletionsPads" sheetId="3" r:id="rId5"/>
     <sheet name="SWDSites" sheetId="4" r:id="rId6"/>
-    <sheet name="FreshwaterSources" sheetId="35" r:id="rId7"/>
+    <sheet name="ExternalWaterSources" sheetId="35" r:id="rId7"/>
     <sheet name="WaterQualityComponents" sheetId="75" r:id="rId8"/>
     <sheet name="StorageSites" sheetId="36" r:id="rId9"/>
     <sheet name="TreatmentSites" sheetId="37" r:id="rId10"/>
@@ -42,7 +42,7 @@
     <sheet name="FlowbackRates" sheetId="58" r:id="rId27"/>
     <sheet name="DisposalCapacity" sheetId="46" r:id="rId28"/>
     <sheet name="TreatmentCapacity" sheetId="62" r:id="rId29"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId30"/>
+    <sheet name="ExtWaterSourcingAvailability" sheetId="47" r:id="rId30"/>
     <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId31"/>
     <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId32"/>
     <sheet name="ProductionTankCapacity" sheetId="61" r:id="rId33"/>
@@ -50,12 +50,12 @@
     <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId35"/>
     <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId36"/>
     <sheet name="PipelineOperationalCost" sheetId="54" r:id="rId37"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId38"/>
+    <sheet name="ExternalSourcingCost" sheetId="52" r:id="rId38"/>
     <sheet name="PadStorageCost" sheetId="70" r:id="rId39"/>
     <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId40"/>
     <sheet name="TruckingTime" sheetId="7" r:id="rId41"/>
     <sheet name="TreatmentEfficiency" sheetId="69" r:id="rId42"/>
-    <sheet name="FreshwaterQuality" sheetId="76" r:id="rId43"/>
+    <sheet name="ExternalWaterQuality" sheetId="76" r:id="rId43"/>
     <sheet name="PadWaterQuality" sheetId="71" r:id="rId44"/>
     <sheet name="StorageInitialWaterQuality" sheetId="72" r:id="rId45"/>
   </sheets>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="163">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -200,12 +200,6 @@
     <t>Forecasted disposal capacity</t>
   </si>
   <si>
-    <t>Freshwater Costs</t>
-  </si>
-  <si>
-    <t>Cost for sourcing freshwater for frac</t>
-  </si>
-  <si>
     <t>Disposal Costs</t>
   </si>
   <si>
@@ -314,9 +308,6 @@
     <t>List of all Production Tank Identifiers [-]</t>
   </si>
   <si>
-    <t>List of all Freshwater Source Identifiers [-]</t>
-  </si>
-  <si>
     <t>List of all Storage Site Identifiers [-]</t>
   </si>
   <si>
@@ -329,9 +320,6 @@
     <t>List of all Network Node Identifiers [-]</t>
   </si>
   <si>
-    <t>Freshwater Sources to Completions Pads Piping Arcs [-]</t>
-  </si>
-  <si>
     <t>Production Pads to Completions Pads Trucking Arcs [-]</t>
   </si>
   <si>
@@ -344,9 +332,6 @@
     <t>Production Pads to Production Tanks Links [-]</t>
   </si>
   <si>
-    <t>Freshwater Sources to Completions Pads Trucking Arcs [-]</t>
-  </si>
-  <si>
     <t>Production Pads to Treatment Facilities Trucking Arcs [-]</t>
   </si>
   <si>
@@ -368,9 +353,6 @@
     <t>SWDSites</t>
   </si>
   <si>
-    <t>FreshwaterSources</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -564,6 +546,27 @@
   </si>
   <si>
     <t>List of all Water Quality Components [-]</t>
+  </si>
+  <si>
+    <t>Completions Pads to Completions Pads Trucking Arcs [-]</t>
+  </si>
+  <si>
+    <t>Cost for sourcing external water for frac</t>
+  </si>
+  <si>
+    <t>External Water Costs</t>
+  </si>
+  <si>
+    <t>List of all External Water Source Identifiers [-]</t>
+  </si>
+  <si>
+    <t>External Water Sources to Completions Pads Piping Arcs [-]</t>
+  </si>
+  <si>
+    <t>ExternalWaterSources</t>
+  </si>
+  <si>
+    <t>External Water Sources to Completions Pads Trucking Arcs [-]</t>
   </si>
 </sst>
 </file>
@@ -1328,8 +1331,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6955974" y="1113310"/>
-          <a:ext cx="3166753" cy="4167290"/>
+          <a:off x="6565078" y="1156605"/>
+          <a:ext cx="2931721" cy="4330576"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1342,9 +1345,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1382,7 +1385,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1488,7 +1491,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1630,7 +1633,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1764,7 +1767,7 @@
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
       <c r="C10" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
@@ -2066,12 +2069,12 @@
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="17"/>
       <c r="C31" s="22" t="s">
-        <v>40</v>
+        <v>158</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
       <c r="F31" s="19" t="s">
-        <v>41</v>
+        <v>157</v>
       </c>
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
@@ -2079,18 +2082,18 @@
       <c r="J31" s="19"/>
       <c r="K31" s="20"/>
       <c r="M31" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="17"/>
       <c r="C32" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
@@ -2101,12 +2104,12 @@
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="17"/>
       <c r="C33" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
       <c r="F33" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G33" s="19"/>
       <c r="H33" s="19"/>
@@ -2117,12 +2120,12 @@
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="17"/>
       <c r="C34" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
       <c r="F34" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
@@ -2133,12 +2136,12 @@
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="17"/>
       <c r="C35" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
       <c r="F35" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
@@ -2149,12 +2152,12 @@
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="17"/>
       <c r="C36" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
       <c r="F36" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G36" s="19"/>
       <c r="H36" s="19"/>
@@ -2184,7 +2187,7 @@
     <hyperlink ref="C28" location="FlowbackRates!A1" display="Flowback Rates" xr:uid="{7AB55603-1A43-41A6-9693-1B89B6DCD5C2}"/>
     <hyperlink ref="C29" location="ProductionRates!A1" display="Production Rates" xr:uid="{60EE3CB2-6945-4EF9-994B-D4937DBB327B}"/>
     <hyperlink ref="C30" location="DisposalCapacity!A1" display="Disposal Capacity" xr:uid="{CAE3DFDA-8B08-4283-9205-309B32142AC6}"/>
-    <hyperlink ref="C31" location="FreshwaterCost!A1" display="Freshwater Costs" xr:uid="{88138AE4-1159-418A-A895-39D1A4152B0C}"/>
+    <hyperlink ref="C31" location="ExternalSourcingCost!A1" display="External Water Costs" xr:uid="{88138AE4-1159-418A-A895-39D1A4152B0C}"/>
     <hyperlink ref="C32" location="ReuseCost!A1" display="Reuse Costs" xr:uid="{146BA03C-3C08-4957-9F2D-51584E8F9494}"/>
     <hyperlink ref="C33" location="DisposalCost!A1" display="Disposal Costs" xr:uid="{906CEF7C-3D67-4EB0-9995-1E45CB542C7C}"/>
     <hyperlink ref="C34" location="HaulingRates!A1" display="Hauling Rates" xr:uid="{E573813D-C46B-4CBC-BD31-9C5E10AF7D7A}"/>
@@ -2222,17 +2225,17 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -2270,7 +2273,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -2314,7 +2317,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -2351,12 +2354,12 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>8</v>
@@ -2367,7 +2370,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -2376,7 +2379,7 @@
     </row>
     <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -2397,24 +2400,24 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" style="1" customWidth="1"/>
     <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>160</v>
       </c>
       <c r="B1" s="39"/>
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -2425,18 +2428,18 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="36">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
@@ -2463,7 +2466,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2486,7 +2489,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2513,13 +2516,13 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E1" s="39"/>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -2583,22 +2586,23 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="25.42578125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -2606,7 +2610,7 @@
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="36">
         <v>1</v>
@@ -2614,7 +2618,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
@@ -2634,22 +2638,23 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="19.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -2704,21 +2709,21 @@
   <sheetData>
     <row r="1" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:53" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E2" s="47" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F2" s="48"/>
       <c r="G2" s="48"/>
@@ -2729,52 +2734,52 @@
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E3" s="53" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F3" s="54" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G3" s="55" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H3" s="56"/>
       <c r="I3" s="55" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="J3" s="54" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K3" s="57" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F4" s="54" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G4" s="55" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H4" s="56"/>
       <c r="I4" s="55"/>
@@ -2783,13 +2788,13 @@
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E5" s="58"/>
       <c r="F5" s="59"/>
@@ -2801,22 +2806,22 @@
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F6" s="54" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G6" s="55" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H6" s="52"/>
       <c r="I6" s="59"/>
@@ -2825,22 +2830,22 @@
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F7" s="54" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G7" s="55" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H7" s="52"/>
       <c r="I7" s="59"/>
@@ -2849,13 +2854,13 @@
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E8" s="58"/>
       <c r="F8" s="59"/>
@@ -2865,87 +2870,87 @@
       <c r="J8" s="59"/>
       <c r="K8" s="60"/>
       <c r="AT8" s="37" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="AU8" s="37" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="AV8" s="37" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="AW8" s="37" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="AX8" s="37" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="AY8" s="37" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="AZ8" s="37" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="BA8" s="37" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E9" s="58" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F9" s="59" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G9" s="59" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="H9" s="52"/>
       <c r="I9" s="59"/>
       <c r="J9" s="59"/>
       <c r="K9" s="60"/>
       <c r="AT9" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="AU9" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="AV9" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="AW9" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="AX9" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="AY9" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="AZ9" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="BA9" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E10" s="58"/>
       <c r="F10" s="59"/>
@@ -2955,72 +2960,72 @@
       <c r="J10" s="59"/>
       <c r="K10" s="60"/>
       <c r="AT10" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="AU10" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="AV10" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="AW10" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="AX10" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="AY10" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="AZ10" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="BA10" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B11" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="61" t="s">
+        <v>137</v>
+      </c>
+      <c r="E11" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="D11" s="61" t="s">
-        <v>143</v>
-      </c>
-      <c r="E11" s="62" t="s">
-        <v>144</v>
-      </c>
       <c r="F11" s="63" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G11" s="64" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="H11" s="61"/>
       <c r="I11" s="65" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="J11" s="63" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K11" s="64" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AU11" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="BA11" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="AU12" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="BA12" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3074,18 +3079,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3159,15 +3164,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3203,60 +3208,60 @@
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="O2" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="O2" s="27" t="s">
-        <v>74</v>
-      </c>
       <c r="P2" s="7" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="Q2" s="27" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3451,22 +3456,22 @@
     </row>
     <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="27" t="s">
         <v>58</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3526,25 +3531,25 @@
     </row>
     <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="27" t="s">
         <v>58</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -3552,7 +3557,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" s="9">
         <v>1058</v>
@@ -3575,7 +3580,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C4" s="9">
         <v>1058</v>
@@ -3598,7 +3603,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" s="9">
         <v>466</v>
@@ -3621,7 +3626,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6" s="9">
         <v>466</v>
@@ -3644,7 +3649,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C7" s="9">
         <v>466</v>
@@ -3667,7 +3672,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C8" s="9">
         <v>200</v>
@@ -3690,7 +3695,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9" s="9">
         <v>200</v>
@@ -3713,7 +3718,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" s="9">
         <v>200</v>
@@ -3736,7 +3741,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11" s="9">
         <v>200</v>
@@ -3759,7 +3764,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12" s="9">
         <v>331</v>
@@ -3782,7 +3787,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="9">
         <v>331</v>
@@ -3805,7 +3810,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" s="9">
         <v>331</v>
@@ -3828,7 +3833,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" s="9">
         <v>895</v>
@@ -3851,7 +3856,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" s="10">
         <v>895</v>
@@ -3903,22 +3908,22 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="27" t="s">
         <v>58</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -4057,25 +4062,25 @@
     </row>
     <row r="2" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="27" t="s">
         <v>58</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4083,7 +4088,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="69" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C3" s="10">
         <v>250</v>
@@ -4106,7 +4111,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="69" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C4" s="10">
         <v>250</v>
@@ -4158,22 +4163,22 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="27" t="s">
         <v>58</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4229,16 +4234,16 @@
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" s="36">
         <v>5000</v>
@@ -4246,7 +4251,7 @@
     </row>
     <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="11">
         <v>10000</v>
@@ -4360,43 +4365,45 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" style="1" customWidth="1"/>
     <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Availability"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Freshwater Sourcing Availability [bbl/day]</v>
+        <f>_xlfn.CONCAT( "Table of External Water Sourcing Availability"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of External Water Sourcing Availability [bbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="27" t="s">
         <v>58</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="9">
         <v>30000</v>
@@ -4416,7 +4423,7 @@
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="10">
         <v>20000</v>
@@ -4466,22 +4473,22 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="27" t="s">
         <v>58</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4533,10 +4540,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4582,9 +4589,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4599,15 +4604,15 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" s="36">
         <v>9</v>
@@ -4615,7 +4620,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="11">
         <v>8</v>
@@ -4669,10 +4674,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4697,7 +4702,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4713,7 +4718,7 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -4721,7 +4726,7 @@
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="36">
         <v>0.75</v>
@@ -4729,7 +4734,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="11">
         <v>0.85</v>
@@ -4748,33 +4753,31 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" style="1" customWidth="1"/>
     <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Freshwater Sourcing Cost [USD/bbl]</v>
+        <f>_xlfn.CONCAT( "Table of External Water Sourcing Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of External Water Sourcing Cost [USD/bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="36">
         <v>0.25</v>
@@ -4782,7 +4785,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="11">
         <v>0.5</v>
@@ -4819,22 +4822,22 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="27" t="s">
         <v>58</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -4888,28 +4891,28 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D4" s="12"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
@@ -4917,62 +4920,62 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -5006,10 +5009,10 @@
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>92</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -5022,7 +5025,7 @@
     </row>
     <row r="4" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="36">
         <v>88</v>
@@ -5030,7 +5033,7 @@
     </row>
     <row r="5" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" s="36">
         <v>89</v>
@@ -5108,7 +5111,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>3</v>
@@ -5129,10 +5132,10 @@
         <v>8</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5241,7 +5244,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -5256,7 +5259,7 @@
     </row>
     <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -5271,7 +5274,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -5284,7 +5287,7 @@
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -5322,20 +5325,20 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B3" s="36">
         <v>1</v>
@@ -5343,7 +5346,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
@@ -5368,27 +5371,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Water Quality of Freshwater Sources [",VLOOKUP("concentration", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Water Quality of Freshwater Sources [mg/liter]</v>
+        <f>_xlfn.CONCAT( "Table of Water Quality of External Water Sources [",VLOOKUP("concentration", Units!$A$2:$B$11, 2, FALSE),"]")</f>
+        <v>Table of Water Quality of External Water Sources [mg/liter]</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="70">
         <v>0</v>
@@ -5396,7 +5399,7 @@
     </row>
     <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="71">
         <v>0</v>
@@ -5432,10 +5435,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -5517,10 +5520,10 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5608,12 +5611,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -5649,17 +5652,17 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -5690,12 +5693,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -5729,7 +5732,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implement water quality for externally sourced water (strategic and operational models) (#286)
* Implement water quality for freshwater sources

* Implement freshwater quality for operational model

* Change all references to fresh water to external water

* Run black
</commit_message>
<xml_diff>
--- a/pareto/case_studies/operational_generic_case_study.xlsx
+++ b/pareto/case_studies/operational_generic_case_study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\melodys\Documents\1. Projects\PARETO - Department of Energy\Code Updates\GIT Tracked Folder\project-pareto\pareto\case_studies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E48321-923B-48F5-8BE6-3E12B24E4753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CE4AC1-C8F3-4047-87A2-883EE564938B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="770" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="770" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -19,43 +19,45 @@
     <sheet name="ProductionTanks" sheetId="34" r:id="rId4"/>
     <sheet name="CompletionsPads" sheetId="3" r:id="rId5"/>
     <sheet name="SWDSites" sheetId="4" r:id="rId6"/>
-    <sheet name="FreshwaterSources" sheetId="35" r:id="rId7"/>
-    <sheet name="StorageSites" sheetId="36" r:id="rId8"/>
-    <sheet name="TreatmentSites" sheetId="37" r:id="rId9"/>
-    <sheet name="ReuseOptions" sheetId="38" r:id="rId10"/>
-    <sheet name="NetworkNodes" sheetId="39" r:id="rId11"/>
-    <sheet name="RCA" sheetId="67" r:id="rId12"/>
-    <sheet name="FCA" sheetId="41" r:id="rId13"/>
-    <sheet name="PRT" sheetId="59" r:id="rId14"/>
-    <sheet name="CRT" sheetId="60" r:id="rId15"/>
-    <sheet name="PCT" sheetId="42" r:id="rId16"/>
-    <sheet name="FCT" sheetId="53" r:id="rId17"/>
-    <sheet name="CCT" sheetId="57" r:id="rId18"/>
-    <sheet name="PKT" sheetId="43" r:id="rId19"/>
-    <sheet name="CKT" sheetId="44" r:id="rId20"/>
-    <sheet name="PAL" sheetId="45" r:id="rId21"/>
-    <sheet name="CompletionsDemand" sheetId="8" r:id="rId22"/>
-    <sheet name="ProductionRates" sheetId="40" r:id="rId23"/>
-    <sheet name="PadRates" sheetId="56" r:id="rId24"/>
-    <sheet name="TankFlowbackRates" sheetId="74" r:id="rId25"/>
-    <sheet name="FlowbackRates" sheetId="58" r:id="rId26"/>
-    <sheet name="DisposalCapacity" sheetId="46" r:id="rId27"/>
-    <sheet name="TreatmentCapacity" sheetId="62" r:id="rId28"/>
-    <sheet name="FreshwaterSourcingAvailability" sheetId="47" r:id="rId29"/>
-    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId30"/>
-    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId31"/>
-    <sheet name="ProductionTankCapacity" sheetId="61" r:id="rId32"/>
-    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId33"/>
-    <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId34"/>
-    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId35"/>
-    <sheet name="PipelineOperationalCost" sheetId="54" r:id="rId36"/>
-    <sheet name="FreshSourcingCost" sheetId="52" r:id="rId37"/>
-    <sheet name="PadStorageCost" sheetId="70" r:id="rId38"/>
-    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId39"/>
-    <sheet name="TruckingTime" sheetId="7" r:id="rId40"/>
-    <sheet name="TreatmentEfficiency" sheetId="69" r:id="rId41"/>
-    <sheet name="PadWaterQuality" sheetId="71" r:id="rId42"/>
-    <sheet name="StorageInitialWaterQuality" sheetId="72" r:id="rId43"/>
+    <sheet name="ExternalWaterSources" sheetId="35" r:id="rId7"/>
+    <sheet name="WaterQualityComponents" sheetId="75" r:id="rId8"/>
+    <sheet name="StorageSites" sheetId="36" r:id="rId9"/>
+    <sheet name="TreatmentSites" sheetId="37" r:id="rId10"/>
+    <sheet name="ReuseOptions" sheetId="38" r:id="rId11"/>
+    <sheet name="NetworkNodes" sheetId="39" r:id="rId12"/>
+    <sheet name="RCA" sheetId="67" r:id="rId13"/>
+    <sheet name="FCA" sheetId="41" r:id="rId14"/>
+    <sheet name="PRT" sheetId="59" r:id="rId15"/>
+    <sheet name="CRT" sheetId="60" r:id="rId16"/>
+    <sheet name="PCT" sheetId="42" r:id="rId17"/>
+    <sheet name="FCT" sheetId="53" r:id="rId18"/>
+    <sheet name="CCT" sheetId="57" r:id="rId19"/>
+    <sheet name="PKT" sheetId="43" r:id="rId20"/>
+    <sheet name="CKT" sheetId="44" r:id="rId21"/>
+    <sheet name="PAL" sheetId="45" r:id="rId22"/>
+    <sheet name="CompletionsDemand" sheetId="8" r:id="rId23"/>
+    <sheet name="ProductionRates" sheetId="40" r:id="rId24"/>
+    <sheet name="PadRates" sheetId="56" r:id="rId25"/>
+    <sheet name="TankFlowbackRates" sheetId="74" r:id="rId26"/>
+    <sheet name="FlowbackRates" sheetId="58" r:id="rId27"/>
+    <sheet name="DisposalCapacity" sheetId="46" r:id="rId28"/>
+    <sheet name="TreatmentCapacity" sheetId="62" r:id="rId29"/>
+    <sheet name="ExtWaterSourcingAvailability" sheetId="47" r:id="rId30"/>
+    <sheet name="CompletionsPadStorage" sheetId="55" r:id="rId31"/>
+    <sheet name="PadOffloadingCapacity" sheetId="48" r:id="rId32"/>
+    <sheet name="ProductionTankCapacity" sheetId="61" r:id="rId33"/>
+    <sheet name="DisposalOperationalCost" sheetId="49" r:id="rId34"/>
+    <sheet name="TreatmentOperationalCost" sheetId="66" r:id="rId35"/>
+    <sheet name="ReuseOperationalCost" sheetId="50" r:id="rId36"/>
+    <sheet name="PipelineOperationalCost" sheetId="54" r:id="rId37"/>
+    <sheet name="ExternalSourcingCost" sheetId="52" r:id="rId38"/>
+    <sheet name="PadStorageCost" sheetId="70" r:id="rId39"/>
+    <sheet name="TruckingHourlyCost" sheetId="51" r:id="rId40"/>
+    <sheet name="TruckingTime" sheetId="7" r:id="rId41"/>
+    <sheet name="TreatmentEfficiency" sheetId="69" r:id="rId42"/>
+    <sheet name="ExternalWaterQuality" sheetId="76" r:id="rId43"/>
+    <sheet name="PadWaterQuality" sheetId="71" r:id="rId44"/>
+    <sheet name="StorageInitialWaterQuality" sheetId="72" r:id="rId45"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -76,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="163">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -198,12 +200,6 @@
     <t>Forecasted disposal capacity</t>
   </si>
   <si>
-    <t>Freshwater Costs</t>
-  </si>
-  <si>
-    <t>Cost for sourcing freshwater for frac</t>
-  </si>
-  <si>
     <t>Disposal Costs</t>
   </si>
   <si>
@@ -312,9 +308,6 @@
     <t>List of all Production Tank Identifiers [-]</t>
   </si>
   <si>
-    <t>List of all Freshwater Source Identifiers [-]</t>
-  </si>
-  <si>
     <t>List of all Storage Site Identifiers [-]</t>
   </si>
   <si>
@@ -327,9 +320,6 @@
     <t>List of all Network Node Identifiers [-]</t>
   </si>
   <si>
-    <t>Freshwater Sources to Completions Pads Piping Arcs [-]</t>
-  </si>
-  <si>
     <t>Production Pads to Completions Pads Trucking Arcs [-]</t>
   </si>
   <si>
@@ -342,9 +332,6 @@
     <t>Production Pads to Production Tanks Links [-]</t>
   </si>
   <si>
-    <t>Freshwater Sources to Completions Pads Trucking Arcs [-]</t>
-  </si>
-  <si>
     <t>Production Pads to Treatment Facilities Trucking Arcs [-]</t>
   </si>
   <si>
@@ -366,9 +353,6 @@
     <t>SWDSites</t>
   </si>
   <si>
-    <t>FreshwaterSources</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
@@ -559,6 +543,30 @@
   </si>
   <si>
     <t>B02</t>
+  </si>
+  <si>
+    <t>List of all Water Quality Components [-]</t>
+  </si>
+  <si>
+    <t>Completions Pads to Completions Pads Trucking Arcs [-]</t>
+  </si>
+  <si>
+    <t>Cost for sourcing external water for frac</t>
+  </si>
+  <si>
+    <t>External Water Costs</t>
+  </si>
+  <si>
+    <t>List of all External Water Source Identifiers [-]</t>
+  </si>
+  <si>
+    <t>External Water Sources to Completions Pads Piping Arcs [-]</t>
+  </si>
+  <si>
+    <t>ExternalWaterSources</t>
+  </si>
+  <si>
+    <t>External Water Sources to Completions Pads Trucking Arcs [-]</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1107,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1256,6 +1264,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1317,8 +1331,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6955974" y="1113310"/>
-          <a:ext cx="3166753" cy="4167290"/>
+          <a:off x="6565078" y="1156605"/>
+          <a:ext cx="2931721" cy="4330576"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1331,9 +1345,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1371,7 +1385,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1477,7 +1491,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1619,7 +1633,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1634,15 +1648,15 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.33203125" customWidth="1"/>
-    <col min="10" max="10" width="4.44140625" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4.42578125" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="14"/>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -1654,7 +1668,7 @@
       <c r="J2" s="15"/>
       <c r="K2" s="16"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="17"/>
       <c r="C3" s="18" t="s">
         <v>10</v>
@@ -1668,7 +1682,7 @@
       <c r="J3" s="19"/>
       <c r="K3" s="20"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="17"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
@@ -1680,7 +1694,7 @@
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
       <c r="C5" s="19" t="s">
         <v>16</v>
@@ -1694,7 +1708,7 @@
       <c r="J5" s="19"/>
       <c r="K5" s="20"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="17"/>
       <c r="C6" s="19" t="s">
         <v>14</v>
@@ -1708,7 +1722,7 @@
       <c r="J6" s="19"/>
       <c r="K6" s="20"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="17"/>
       <c r="C7" s="19" t="s">
         <v>11</v>
@@ -1722,7 +1736,7 @@
       <c r="J7" s="19"/>
       <c r="K7" s="20"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="17"/>
       <c r="C8" s="19" t="s">
         <v>12</v>
@@ -1736,7 +1750,7 @@
       <c r="J8" s="19"/>
       <c r="K8" s="20"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="17"/>
       <c r="C9" s="19" t="s">
         <v>13</v>
@@ -1750,10 +1764,10 @@
       <c r="J9" s="19"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
       <c r="C10" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
@@ -1764,7 +1778,7 @@
       <c r="J10" s="19"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="17"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -1776,7 +1790,7 @@
       <c r="J11" s="19"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="17"/>
       <c r="C12" s="19" t="s">
         <v>17</v>
@@ -1790,7 +1804,7 @@
       <c r="J12" s="19"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="17"/>
       <c r="C13" s="19" t="s">
         <v>15</v>
@@ -1804,7 +1818,7 @@
       <c r="J13" s="19"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="17"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -1816,7 +1830,7 @@
       <c r="J14" s="19"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="17"/>
       <c r="C15" s="19" t="s">
         <v>18</v>
@@ -1830,7 +1844,7 @@
       <c r="J15" s="19"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="17"/>
       <c r="C16" s="19" t="s">
         <v>19</v>
@@ -1844,7 +1858,7 @@
       <c r="J16" s="19"/>
       <c r="K16" s="20"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="17"/>
       <c r="C17" s="19" t="s">
         <v>20</v>
@@ -1858,7 +1872,7 @@
       <c r="J17" s="19"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="17"/>
       <c r="C18" s="19" t="s">
         <v>21</v>
@@ -1872,7 +1886,7 @@
       <c r="J18" s="19"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="17"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -1884,7 +1898,7 @@
       <c r="J19" s="19"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="17"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
@@ -1896,7 +1910,7 @@
       <c r="J20" s="19"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="17"/>
       <c r="C21" s="21" t="s">
         <v>22</v>
@@ -1912,7 +1926,7 @@
       <c r="J21" s="19"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="17"/>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
@@ -1924,7 +1938,7 @@
       <c r="J22" s="19"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="17"/>
       <c r="C23" s="22" t="s">
         <v>24</v>
@@ -1940,7 +1954,7 @@
       <c r="J23" s="19"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="17"/>
       <c r="C24" s="22" t="s">
         <v>25</v>
@@ -1956,7 +1970,7 @@
       <c r="J24" s="19"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="17"/>
       <c r="C25" s="22" t="s">
         <v>26</v>
@@ -1972,7 +1986,7 @@
       <c r="J25" s="19"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="17"/>
       <c r="C26" s="22" t="s">
         <v>30</v>
@@ -1988,7 +2002,7 @@
       <c r="J26" s="19"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="17"/>
       <c r="C27" s="22" t="s">
         <v>32</v>
@@ -2004,7 +2018,7 @@
       <c r="J27" s="19"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="17"/>
       <c r="C28" s="22" t="s">
         <v>34</v>
@@ -2020,7 +2034,7 @@
       <c r="J28" s="19"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="17"/>
       <c r="C29" s="22" t="s">
         <v>35</v>
@@ -2036,7 +2050,7 @@
       <c r="J29" s="19"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="17"/>
       <c r="C30" s="22" t="s">
         <v>38</v>
@@ -2052,15 +2066,15 @@
       <c r="J30" s="19"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="17"/>
       <c r="C31" s="22" t="s">
-        <v>40</v>
+        <v>158</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
       <c r="F31" s="19" t="s">
-        <v>41</v>
+        <v>157</v>
       </c>
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
@@ -2068,18 +2082,18 @@
       <c r="J31" s="19"/>
       <c r="K31" s="20"/>
       <c r="M31" s="26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="17"/>
       <c r="C32" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
@@ -2087,15 +2101,15 @@
       <c r="J32" s="19"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="17"/>
       <c r="C33" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
       <c r="F33" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G33" s="19"/>
       <c r="H33" s="19"/>
@@ -2103,15 +2117,15 @@
       <c r="J33" s="19"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="17"/>
       <c r="C34" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
       <c r="F34" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
@@ -2119,15 +2133,15 @@
       <c r="J34" s="19"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="17"/>
       <c r="C35" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
       <c r="F35" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
@@ -2135,15 +2149,15 @@
       <c r="J35" s="19"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="17"/>
       <c r="C36" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
       <c r="F36" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G36" s="19"/>
       <c r="H36" s="19"/>
@@ -2151,7 +2165,7 @@
       <c r="J36" s="19"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="23"/>
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
@@ -2173,7 +2187,7 @@
     <hyperlink ref="C28" location="FlowbackRates!A1" display="Flowback Rates" xr:uid="{7AB55603-1A43-41A6-9693-1B89B6DCD5C2}"/>
     <hyperlink ref="C29" location="ProductionRates!A1" display="Production Rates" xr:uid="{60EE3CB2-6945-4EF9-994B-D4937DBB327B}"/>
     <hyperlink ref="C30" location="DisposalCapacity!A1" display="Disposal Capacity" xr:uid="{CAE3DFDA-8B08-4283-9205-309B32142AC6}"/>
-    <hyperlink ref="C31" location="FreshwaterCost!A1" display="Freshwater Costs" xr:uid="{88138AE4-1159-418A-A895-39D1A4152B0C}"/>
+    <hyperlink ref="C31" location="ExternalSourcingCost!A1" display="External Water Costs" xr:uid="{88138AE4-1159-418A-A895-39D1A4152B0C}"/>
     <hyperlink ref="C32" location="ReuseCost!A1" display="Reuse Costs" xr:uid="{146BA03C-3C08-4957-9F2D-51584E8F9494}"/>
     <hyperlink ref="C33" location="DisposalCost!A1" display="Disposal Costs" xr:uid="{906CEF7C-3D67-4EB0-9995-1E45CB542C7C}"/>
     <hyperlink ref="C34" location="HaulingRates!A1" display="Hauling Rates" xr:uid="{E573813D-C46B-4CBC-BD31-9C5E10AF7D7A}"/>
@@ -2186,6 +2200,54 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF69D0FC-C70F-430B-9882-945A087A2D92}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:P3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A85E027-57F4-45A3-888B-4C0E11BBDC89}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2196,28 +2258,28 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.33203125" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.33203125" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -2229,7 +2291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F8A809-1347-42CB-A460-105FB2B000F6}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2240,28 +2302,28 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.33203125" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.33203125" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -2273,7 +2335,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19482E4D-5604-4B83-9F7A-0225AC5DE7E0}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2284,20 +2346,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="14.42578125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>8</v>
@@ -2306,18 +2368,18 @@
       <c r="D2" s="7"/>
       <c r="E2" s="27"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="36"/>
     </row>
-    <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -2330,7 +2392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC2D47-F187-4A8D-891B-85F0F5A9A73D}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2338,24 +2400,24 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="25.42578125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>160</v>
       </c>
       <c r="B1" s="39"/>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
@@ -2364,20 +2426,20 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="36">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
@@ -2389,7 +2451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC3797B-8D14-4FB6-B72A-3C0C4341EC79}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2400,11 +2462,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2412,7 +2474,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F1A6821-D55E-4269-AC7B-EA9C0F0EC2AD}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2423,11 +2485,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2435,7 +2497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6ED8ED-0A77-4974-A7C2-D2B875DA1401}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2446,27 +2508,27 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E1" s="39"/>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
@@ -2474,7 +2536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -2482,7 +2544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2490,7 +2552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -2498,7 +2560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -2506,7 +2568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" s="39"/>
     </row>
   </sheetData>
@@ -2516,7 +2578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED7A596-FF30-4282-98C8-7AB378F1FE03}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2524,38 +2586,39 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="25.42578125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
@@ -2567,7 +2630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16082D3-6CFF-4538-9513-170B327E5C50}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -2575,118 +2638,33 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="19.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="11">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AE275C-BC38-44C0-8EFB-EA0A3ABCF1EE}">
-  <sheetPr>
-    <tabColor theme="9" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.88671875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="36"/>
-    </row>
-    <row r="4" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="11">
         <v>1</v>
       </c>
     </row>
@@ -2707,45 +2685,45 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="92.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="0.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="48" width="9.33203125" style="1"/>
-    <col min="49" max="49" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="92.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="0.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="48" width="9.28515625" style="1"/>
+    <col min="49" max="49" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:53" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:53" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E2" s="47" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F2" s="48"/>
       <c r="G2" s="48"/>
@@ -2754,69 +2732,69 @@
       <c r="J2" s="48"/>
       <c r="K2" s="50"/>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E3" s="53" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F3" s="54" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G3" s="55" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H3" s="56"/>
       <c r="I3" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="K3" s="57" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="55" t="s">
         <v>118</v>
-      </c>
-      <c r="J3" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="K3" s="57" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4" s="51" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" s="52" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" s="53" t="s">
-        <v>123</v>
-      </c>
-      <c r="F4" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="G4" s="55" t="s">
-        <v>124</v>
       </c>
       <c r="H4" s="56"/>
       <c r="I4" s="55"/>
       <c r="J4" s="55"/>
       <c r="K4" s="57"/>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E5" s="58"/>
       <c r="F5" s="59"/>
@@ -2826,63 +2804,63 @@
       <c r="J5" s="59"/>
       <c r="K5" s="60"/>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F6" s="54" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G6" s="55" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H6" s="52"/>
       <c r="I6" s="59"/>
       <c r="J6" s="59"/>
       <c r="K6" s="60"/>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F7" s="54" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G7" s="55" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H7" s="52"/>
       <c r="I7" s="59"/>
       <c r="J7" s="59"/>
       <c r="K7" s="60"/>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E8" s="58"/>
       <c r="F8" s="59"/>
@@ -2892,87 +2870,87 @@
       <c r="J8" s="59"/>
       <c r="K8" s="60"/>
       <c r="AT8" s="37" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="AU8" s="37" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="AV8" s="37" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="AW8" s="37" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="AX8" s="37" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="AY8" s="37" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="AZ8" s="37" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="BA8" s="37" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E9" s="58" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F9" s="59" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G9" s="59" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="H9" s="52"/>
       <c r="I9" s="59"/>
       <c r="J9" s="59"/>
       <c r="K9" s="60"/>
       <c r="AT9" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="AU9" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="AV9" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="AW9" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="AX9" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="AY9" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="AZ9" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="BA9" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E10" s="58"/>
       <c r="F10" s="59"/>
@@ -2982,72 +2960,72 @@
       <c r="J10" s="59"/>
       <c r="K10" s="60"/>
       <c r="AT10" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="AU10" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="AV10" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="AW10" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="AX10" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AY10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AZ10" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="BA10" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="AY10" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AZ10" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="BA10" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="33" t="s">
-        <v>141</v>
-      </c>
       <c r="B11" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="61" t="s">
+        <v>137</v>
+      </c>
+      <c r="E11" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="D11" s="61" t="s">
-        <v>143</v>
-      </c>
-      <c r="E11" s="62" t="s">
-        <v>144</v>
-      </c>
       <c r="F11" s="63" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G11" s="64" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="H11" s="61"/>
       <c r="I11" s="65" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="J11" s="63" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K11" s="64" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AU11" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="BA11" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="AU12" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="BA12" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3083,6 +3061,92 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AE275C-BC38-44C0-8EFB-EA0A3ABCF1EE}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="36"/>
+    </row>
+    <row r="4" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="37"/>
+      <c r="C6" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90457C74-863B-4C67-B58B-571271FAEA0E}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -3093,25 +3157,25 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -3125,7 +3189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABD83BE-FC18-4B07-A835-FE113535C483}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -3136,71 +3200,71 @@
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="O2" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="O2" s="27" t="s">
-        <v>74</v>
-      </c>
       <c r="P2" s="7" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="Q2" s="27" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
@@ -3225,7 +3289,7 @@
       <c r="P3" s="9"/>
       <c r="Q3" s="36"/>
     </row>
-    <row r="4" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -3252,7 +3316,7 @@
       <c r="P4" s="9"/>
       <c r="Q4" s="36"/>
     </row>
-    <row r="5" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -3281,7 +3345,7 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="36"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -3308,7 +3372,7 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="36"/>
     </row>
-    <row r="7" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -3333,7 +3397,7 @@
       <c r="P7" s="10"/>
       <c r="Q7" s="11"/>
     </row>
-    <row r="8" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
@@ -3365,7 +3429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6FA210-6C83-4CC4-AF45-F41CDC53F769}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3376,41 +3440,41 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="9.33203125" style="1"/>
+    <col min="1" max="7" width="9.28515625" style="1"/>
     <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.33203125" style="1"/>
+    <col min="9" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B11, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
         <v>Table of Completions Water Demand for Completions Sites over days [bbl/day]</v>
       </c>
       <c r="H1" s="39"/>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -3430,7 +3494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F8" s="12"/>
     </row>
   </sheetData>
@@ -3440,7 +3504,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF09514F-DAFF-4764-9C34-8E43F32C86F9}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3451,49 +3515,49 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="8" customWidth="1"/>
     <col min="2" max="2" width="23" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.33203125" style="1"/>
+    <col min="3" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="str">
         <f>_xlfn.CONCAT( "Table of Production Rate Forecasts by Tanks and Pads"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Production Rate Forecasts by Tanks and Pads [bbl/day]</v>
       </c>
       <c r="B1" s="39"/>
     </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" s="9">
         <v>1058</v>
@@ -3511,12 +3575,12 @@
         <v>996</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C4" s="9">
         <v>1058</v>
@@ -3534,12 +3598,12 @@
         <v>996</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" s="9">
         <v>466</v>
@@ -3557,12 +3621,12 @@
         <v>455</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6" s="9">
         <v>466</v>
@@ -3580,12 +3644,12 @@
         <v>455</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C7" s="9">
         <v>466</v>
@@ -3603,12 +3667,12 @@
         <v>455</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C8" s="9">
         <v>200</v>
@@ -3626,12 +3690,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9" s="9">
         <v>200</v>
@@ -3649,12 +3713,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" s="9">
         <v>200</v>
@@ -3672,12 +3736,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11" s="9">
         <v>200</v>
@@ -3695,12 +3759,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C12" s="9">
         <v>331</v>
@@ -3718,12 +3782,12 @@
         <v>329</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="9">
         <v>331</v>
@@ -3741,12 +3805,12 @@
         <v>329</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" s="9">
         <v>331</v>
@@ -3764,12 +3828,12 @@
         <v>329</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C15" s="9">
         <v>895</v>
@@ -3787,12 +3851,12 @@
         <v>883</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" s="10">
         <v>895</v>
@@ -3810,7 +3874,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G21" s="12"/>
     </row>
   </sheetData>
@@ -3819,7 +3883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AE5548-F8CC-426B-BF72-21E59575CB18}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3830,39 +3894,39 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" style="8" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="17.140625" style="8" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="str">
         <f>_xlfn.CONCAT( "Table of Production Rate Forecasts by Pads"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Production Rate Forecasts by Pads [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
@@ -3882,7 +3946,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -3902,7 +3966,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -3922,7 +3986,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -3942,7 +4006,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>7</v>
       </c>
@@ -3962,7 +4026,7 @@
         <v>1766</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F12" s="12"/>
     </row>
   </sheetData>
@@ -3971,7 +4035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1F3225-05BE-4B0D-AE83-9F04DDDFE920}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -3982,49 +4046,49 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="9.33203125" style="1"/>
+    <col min="1" max="8" width="9.28515625" style="1"/>
     <col min="9" max="9" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.33203125" style="1"/>
+    <col min="10" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B11, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
         <v>Table of Completions Water Demand for Completions Sites over days [bbl/day]</v>
       </c>
       <c r="I1" s="39"/>
     </row>
-    <row r="2" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="69" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C3" s="10">
         <v>250</v>
@@ -4042,12 +4106,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="69" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C4" s="10">
         <v>250</v>
@@ -4065,7 +4129,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G8" s="12"/>
     </row>
   </sheetData>
@@ -4074,7 +4138,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16A47F7-A2FF-4DEE-B278-2DA8AB93D602}">
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
@@ -4085,39 +4149,39 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="8"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="9.28515625" style="8"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="str">
         <f>_xlfn.CONCAT( "Table of Flowback Rate Forecasts by Pads"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Flowback Rate Forecasts by Pads [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4137,7 +4201,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F8" s="12"/>
     </row>
   </sheetData>
@@ -4146,7 +4210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D65BC4-7454-4A45-AA93-771B11A13108}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4155,12 +4219,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Initial Disposal Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Initial Disposal Capacity [bbl/day]</v>
@@ -4168,33 +4232,33 @@
       <c r="B1" s="39"/>
       <c r="D1" s="39"/>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D2" s="39"/>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" s="36">
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="11">
         <v>10000</v>
       </c>
       <c r="D4" s="39"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="39"/>
       <c r="B6" s="39"/>
       <c r="D6" s="39"/>
@@ -4205,7 +4269,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59865970-D83F-46CB-8781-62CE35DBF4B5}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4214,9 +4278,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Table of Reuse Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Reuse Capacity [bbl/day]</v>
@@ -4224,96 +4288,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
-  <sheetPr>
-    <tabColor rgb="FFD9C6FE"/>
-  </sheetPr>
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Availability"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Freshwater Sourcing Availability [bbl/day]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="9">
-        <v>30000</v>
-      </c>
-      <c r="C3" s="9">
-        <v>30000</v>
-      </c>
-      <c r="D3" s="9">
-        <v>30000</v>
-      </c>
-      <c r="E3" s="9">
-        <v>30000</v>
-      </c>
-      <c r="F3" s="36">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="10">
-        <v>20000</v>
-      </c>
-      <c r="C4" s="10">
-        <v>20000</v>
-      </c>
-      <c r="D4" s="10">
-        <v>20000</v>
-      </c>
-      <c r="E4" s="10">
-        <v>20000</v>
-      </c>
-      <c r="F4" s="11">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F9" s="12"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4328,39 +4302,39 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="9.33203125" style="1"/>
-    <col min="10" max="10" width="11.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="4.5546875" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="9" width="9.28515625" style="1"/>
+    <col min="10" max="10" width="11.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="39"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="39"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -4368,12 +4342,12 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="39"/>
       <c r="C10" s="39"/>
     </row>
@@ -4385,6 +4359,98 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A2DBF7-A8C0-4CE1-BE66-F8E077B6F0F1}">
+  <sheetPr>
+    <tabColor rgb="FFD9C6FE"/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of External Water Sourcing Availability"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of External Water Sourcing Availability [bbl/day]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="9">
+        <v>30000</v>
+      </c>
+      <c r="C3" s="9">
+        <v>30000</v>
+      </c>
+      <c r="D3" s="9">
+        <v>30000</v>
+      </c>
+      <c r="E3" s="9">
+        <v>30000</v>
+      </c>
+      <c r="F3" s="36">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="10">
+        <v>20000</v>
+      </c>
+      <c r="C4" s="10">
+        <v>20000</v>
+      </c>
+      <c r="D4" s="10">
+        <v>20000</v>
+      </c>
+      <c r="E4" s="10">
+        <v>20000</v>
+      </c>
+      <c r="F4" s="11">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA48CF8D-5373-4539-A55F-3258FEB20DFB}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4393,39 +4459,39 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="15.140625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Completions Pad Storage Capacity [bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4451,7 +4517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F216C6A0-7BAD-498F-AAE7-F43EE79415DD}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4460,27 +4526,27 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Pad Offloading Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Pad Offloading Capacity [bbl/day]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4494,7 +4560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EB27A2-91E8-4B14-8B2B-D8903B8CA8E8}">
   <sheetPr>
     <tabColor rgb="FFD9C6FE"/>
@@ -4503,9 +4569,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Production Tank Capacity"," [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Production Tank Capacity [bbl]</v>
@@ -4516,47 +4582,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDED9A13-6613-4A4D-92BC-DD0B79B273AD}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Disposal Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Disposal Operational Cost [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" s="36">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="11">
         <v>8</v>
@@ -4568,7 +4632,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74013BD9-1426-4BFB-8D02-5A2A33597048}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4579,13 +4643,13 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F35D225-B5AF-4E75-9547-7AC1A8034351}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4596,27 +4660,27 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Reuse Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Reuse Operational Cost [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>8</v>
       </c>
@@ -4630,7 +4694,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FF3D68-9420-4DF5-8A14-DD803657C7A5}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4638,95 +4702,42 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Piping Operational Costs [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Piping Operational Costs [USD/bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="36">
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="11">
         <v>0.85</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.5546875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Freshwater Sourcing Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
-        <v>Table of Freshwater Sourcing Cost [USD/bbl]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="36">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="11">
-        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -4736,6 +4747,57 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B9AF2E-9304-4DC1-ABFA-7D5DAA6BA0BC}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of External Water Sourcing Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
+        <v>Table of External Water Sourcing Cost [USD/bbl]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="36">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2915391D-1D4E-446C-B6C1-F25D75A5D98F}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -4746,39 +4808,39 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.33203125" style="1"/>
+    <col min="2" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity over Time [",VLOOKUP("volume", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Completions Pad Storage Capacity over Time [bbl]</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B2" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -4796,106 +4858,6 @@
       </c>
       <c r="F3" s="42">
         <v>250</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Trucking Hourly Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", "hour","]")</f>
-        <v>Table of Trucking Hourly Cost [USD/hour]</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="36">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="36">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5" s="36">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="36">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="36">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="36">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="36">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="11">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -4915,105 +4877,105 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.33203125" style="1"/>
-    <col min="3" max="3" width="3.5546875" style="1" customWidth="1"/>
-    <col min="4" max="12" width="9.33203125" style="1"/>
-    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5546875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="2" width="9.28515625" style="1"/>
+    <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
+    <col min="4" max="12" width="9.28515625" style="1"/>
+    <col min="13" max="13" width="11.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5703125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -5024,6 +4986,106 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BECCB21-1375-4BFB-9F09-24B2AEEBDEA4}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Trucking Hourly Cost [",VLOOKUP("currency", Units!$A$2:$B$9, 2, FALSE),"/", "hour","]")</f>
+        <v>Table of Trucking Hourly Cost [USD/hour]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="36">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="36">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="36">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="36">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="36">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="36">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="36">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D257926-ED56-4D32-9A5B-F7129B221F36}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -5034,22 +5096,22 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2" max="6" width="9.33203125" style="1"/>
-    <col min="7" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2" max="6" width="9.28515625" style="1"/>
+    <col min="7" max="8" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>3</v>
@@ -5070,13 +5132,13 @@
         <v>8</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -5093,7 +5155,7 @@
       </c>
       <c r="I3" s="36"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -5112,7 +5174,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -5129,7 +5191,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -5146,7 +5208,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -5163,7 +5225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -5180,9 +5242,9 @@
       </c>
       <c r="I8" s="36"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -5195,9 +5257,9 @@
       <c r="H9" s="9"/>
       <c r="I9" s="36"/>
     </row>
-    <row r="10" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -5210,9 +5272,9 @@
       <c r="H10" s="9"/>
       <c r="I10" s="36"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -5223,9 +5285,9 @@
       <c r="H11" s="9"/>
       <c r="I11" s="36"/>
     </row>
-    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -5236,7 +5298,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="11"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" s="13"/>
     </row>
   </sheetData>
@@ -5245,7 +5307,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4E39D9-E2B5-4E92-A460-6BB588CED0C5}">
   <sheetPr>
     <tabColor rgb="FFAFF3DE"/>
@@ -5256,35 +5318,35 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B3" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B4" s="11">
         <v>1</v>
@@ -5296,7 +5358,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE408470-1FBA-45E4-B7D1-937724BB7595}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Water Quality of External Water Sources [",VLOOKUP("concentration", Units!$A$2:$B$11, 2, FALSE),"]")</f>
+        <v>Table of Water Quality of External Water Sources [mg/liter]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="71">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3E2031-E70C-46E6-B55F-07206AFEE600}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -5307,27 +5421,27 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Table of Water Quality of Produced Water and Flowback Water [",VLOOKUP("concentration", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Water Quality of Produced Water and Flowback Water [mg/liter]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
@@ -5335,7 +5449,7 @@
         <v>142277</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>4</v>
       </c>
@@ -5343,7 +5457,7 @@
         <v>140998</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -5351,7 +5465,7 @@
         <v>172490.2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
@@ -5359,7 +5473,7 @@
         <v>257547</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
         <v>7</v>
       </c>
@@ -5367,7 +5481,7 @@
         <v>241833.8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
@@ -5381,7 +5495,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465369F7-E9A8-4A2B-BBBA-6F1C07C7C51F}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -5392,27 +5506,27 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT( "Table of Initial Water Quality at Storage [",VLOOKUP("concentration", Units!$A$2:$B$9, 2, FALSE),"]")</f>
         <v>Table of Initial Water Quality at Storage [mg/liter]</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="44"/>
       <c r="B3" s="45"/>
     </row>
@@ -5433,30 +5547,30 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.33203125" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.33203125" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
@@ -5479,30 +5593,30 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="4.44140625" style="1" customWidth="1"/>
-    <col min="5" max="14" width="9.33203125" style="1"/>
-    <col min="15" max="15" width="12.109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.5546875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="4.42578125" style="1" customWidth="1"/>
+    <col min="5" max="14" width="9.28515625" style="1"/>
+    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.5703125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -5520,35 +5634,35 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.33203125" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.33203125" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -5562,6 +5676,37 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B022271-250D-45AC-910B-001BCA072919}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0D7E5C-CD82-4DB8-A226-3E1C788BA0DC}">
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -5572,77 +5717,29 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.28515625" style="1"/>
+    <col min="4" max="4" width="3.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.33203125" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.33203125" style="1"/>
+    <col min="6" max="13" width="9.28515625" style="1"/>
+    <col min="14" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF69D0FC-C70F-430B-9882-945A087A2D92}">
-  <sheetPr>
-    <tabColor theme="9" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:P3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="3" width="9.33203125" style="1"/>
-    <col min="4" max="4" width="3.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32" style="1" customWidth="1"/>
-    <col min="6" max="13" width="9.33203125" style="1"/>
-    <col min="14" max="14" width="12.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.33203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>

</xml_diff>

<commit_message>
Fix more tests - change emissions variables to expressions
</commit_message>
<xml_diff>
--- a/pareto/case_studies/operational_generic_case_study.xlsx
+++ b/pareto/case_studies/operational_generic_case_study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CE4AC1-C8F3-4047-87A2-883EE564938B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9840A23E-FA9F-42CA-8FF2-F69546A65F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="770" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="770" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="168">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -567,6 +567,21 @@
   </si>
   <si>
     <t>External Water Sources to Completions Pads Trucking Arcs [-]</t>
+  </si>
+  <si>
+    <t>mass</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>Mass units is used for measuring emissions coefficients (e.g. 10g per treated produced water bbl).</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>1000g</t>
   </si>
 </sst>
 </file>
@@ -2682,7 +2697,7 @@
   <dimension ref="A1:BA12"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2984,33 +2999,33 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="B11" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="D11" s="61" t="s">
+      <c r="B11" s="51" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="E11" s="62" t="s">
+      <c r="E11" s="58" t="s">
         <v>138</v>
       </c>
-      <c r="F11" s="63" t="s">
+      <c r="F11" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="G11" s="64" t="s">
+      <c r="G11" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="H11" s="61"/>
-      <c r="I11" s="65" t="s">
+      <c r="H11" s="52"/>
+      <c r="I11" s="59" t="s">
         <v>140</v>
       </c>
-      <c r="J11" s="63" t="s">
+      <c r="J11" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="K11" s="64" t="s">
+      <c r="K11" s="60" t="s">
         <v>141</v>
       </c>
       <c r="AU11" s="1" t="s">
@@ -3020,7 +3035,29 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="D12" s="61" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="F12" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="H12" s="61"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="64"/>
       <c r="AU12" s="1" t="s">
         <v>117</v>
       </c>
@@ -3048,7 +3085,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{8F8B861C-C393-4435-8DC0-EC8EEEE3BBFD}">
       <formula1>$AT$9:$AT$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{9A2FD3DB-3FAE-4601-8694-0155021F205A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{994F79F2-F31F-4D1D-90CF-A36A61255EFA}">
       <formula1>$BA$9:$BA$12</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{9168A5F5-CA80-4564-8DDA-57F03CF7364B}">
@@ -3450,7 +3487,7 @@
     <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B11, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Completions Water Demand for Completions Sites over days [bbl/day]</v>
+        <v>Table of Completions Water Demand for Completions Sites over weeks [bbl/day]</v>
       </c>
       <c r="H1" s="39"/>
     </row>
@@ -4056,7 +4093,7 @@
     <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B11, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Completions Water Demand for Completions Sites over days [bbl/day]</v>
+        <v>Table of Completions Water Demand for Completions Sites over weeks [bbl/day]</v>
       </c>
       <c r="I1" s="39"/>
     </row>

</xml_diff>

<commit_message>
Fix operational model tests
</commit_message>
<xml_diff>
--- a/pareto/case_studies/operational_generic_case_study.xlsx
+++ b/pareto/case_studies/operational_generic_case_study.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\repos\project-pareto\pareto\case_studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9840A23E-FA9F-42CA-8FF2-F69546A65F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C51834-BEA3-41E6-80F1-B270D268E053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="770" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
@@ -1122,7 +1122,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1283,6 +1283,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3003,29 +3013,30 @@
       <c r="A11" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="B11" s="51" t="s">
-        <v>136</v>
-      </c>
+      <c r="B11" s="72" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="73"/>
       <c r="D11" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="F11" s="59" t="s">
+      <c r="F11" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="G11" s="59" t="s">
+      <c r="G11" s="57" t="s">
         <v>139</v>
       </c>
       <c r="H11" s="52"/>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="J11" s="59" t="s">
+      <c r="J11" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="K11" s="60" t="s">
+      <c r="K11" s="57" t="s">
         <v>141</v>
       </c>
       <c r="AU11" s="1" t="s">
@@ -3085,7 +3096,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{8F8B861C-C393-4435-8DC0-EC8EEEE3BBFD}">
       <formula1>$AT$9:$AT$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{994F79F2-F31F-4D1D-90CF-A36A61255EFA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{9A2FD3DB-3FAE-4601-8694-0155021F205A}">
       <formula1>$BA$9:$BA$12</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{9168A5F5-CA80-4564-8DDA-57F03CF7364B}">
@@ -3487,7 +3498,7 @@
     <row r="1" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B11, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Completions Water Demand for Completions Sites over weeks [bbl/day]</v>
+        <v>Table of Completions Water Demand for Completions Sites over days [bbl/day]</v>
       </c>
       <c r="H1" s="39"/>
     </row>
@@ -4093,7 +4104,7 @@
     <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B11, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Completions Water Demand for Completions Sites over weeks [bbl/day]</v>
+        <v>Table of Completions Water Demand for Completions Sites over days [bbl/day]</v>
       </c>
       <c r="I1" s="39"/>
     </row>

</xml_diff>